<commit_message>
added docs and changes made
</commit_message>
<xml_diff>
--- a/ApiDesignFlightTicketBookingSystem.xlsx
+++ b/ApiDesignFlightTicketBookingSystem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_projects\ChubbWeeklyAssignmentsAndWorks\Week7\Week7Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_projects\ChubbWeeklyAssignmentsAndWorks\Week8\Week8Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E92DE10-9778-4391-9AC6-24792A4D03B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A57067-13E1-4A20-A9AA-877A9777ADC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="136">
   <si>
     <t>NO</t>
   </si>
@@ -410,17 +410,48 @@
   </si>
   <si>
     <t>http://localhost:8765/passenger-service/passenger/deleteById/{id}</t>
+  </si>
+  <si>
+    <t>/auth-service/api/auth/signout</t>
+  </si>
+  <si>
+    <t>/auth-service/api/auth/signup</t>
+  </si>
+  <si>
+    <t>/auth-service/api/auth/signin</t>
+  </si>
+  <si>
+    <t>200 OK</t>
+  </si>
+  <si>
+    <t>{signed out successfully}</t>
+  </si>
+  <si>
+    <t>{"user registered successfully"}</t>
+  </si>
+  <si>
+    <t>{"username":"asritha"</t>
+  </si>
+  <si>
+    <t>"email":"asritha@gmail.com"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -528,6 +559,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF188038"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="13">
@@ -652,63 +689,70 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -927,24 +971,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z797"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="74" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="74" workbookViewId="0">
+      <selection activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="56.21875" customWidth="1"/>
-    <col min="4" max="4" width="46.44140625" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" customWidth="1"/>
-    <col min="7" max="7" width="40.88671875" customWidth="1"/>
-    <col min="8" max="8" width="37.88671875" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="56.1796875" customWidth="1"/>
+    <col min="4" max="4" width="46.453125" customWidth="1"/>
+    <col min="5" max="5" width="37.90625" customWidth="1"/>
+    <col min="6" max="6" width="26.36328125" customWidth="1"/>
+    <col min="7" max="7" width="40.90625" customWidth="1"/>
+    <col min="8" max="8" width="37.90625" customWidth="1"/>
+    <col min="9" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -954,7 +998,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -998,7 +1042,7 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1036,7 +1080,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="46" t="s">
@@ -1072,7 +1116,7 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1104,7 +1148,7 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1136,7 +1180,7 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1168,7 +1212,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1200,7 +1244,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1232,7 +1276,7 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1264,7 +1308,7 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1294,7 +1338,7 @@
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1326,7 +1370,7 @@
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1356,7 +1400,7 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1386,7 +1430,7 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="11">
         <v>2</v>
       </c>
@@ -1424,7 +1468,7 @@
       <c r="Y15" s="11"/>
       <c r="Z15" s="11"/>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -1458,7 +1502,7 @@
       <c r="Y16" s="11"/>
       <c r="Z16" s="11"/>
     </row>
-    <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="14.25" customHeight="1">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1490,7 +1534,7 @@
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
     </row>
-    <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="14.25" customHeight="1">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -1522,7 +1566,7 @@
       <c r="Y18" s="11"/>
       <c r="Z18" s="11"/>
     </row>
-    <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="14.25" customHeight="1">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -1552,7 +1596,7 @@
       <c r="Y19" s="11"/>
       <c r="Z19" s="11"/>
     </row>
-    <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="14.25" customHeight="1">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -1582,7 +1626,7 @@
       <c r="Y20" s="11"/>
       <c r="Z20" s="11"/>
     </row>
-    <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="14.25" customHeight="1">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -1612,7 +1656,7 @@
       <c r="Y21" s="11"/>
       <c r="Z21" s="11"/>
     </row>
-    <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="14.25" customHeight="1">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -1642,7 +1686,7 @@
       <c r="Y22" s="11"/>
       <c r="Z22" s="11"/>
     </row>
-    <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="14.25" customHeight="1">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -1672,7 +1716,7 @@
       <c r="Y23" s="11"/>
       <c r="Z23" s="11"/>
     </row>
-    <row r="24" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="14.25" customHeight="1">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -1702,7 +1746,7 @@
       <c r="Y24" s="11"/>
       <c r="Z24" s="11"/>
     </row>
-    <row r="25" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="14.25" customHeight="1">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -1732,7 +1776,7 @@
       <c r="Y25" s="11"/>
       <c r="Z25" s="11"/>
     </row>
-    <row r="26" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="14.25" customHeight="1">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -1764,7 +1808,7 @@
       <c r="Y26" s="11"/>
       <c r="Z26" s="11"/>
     </row>
-    <row r="27" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="14.25" customHeight="1">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -1792,7 +1836,7 @@
       <c r="Y27" s="11"/>
       <c r="Z27" s="11"/>
     </row>
-    <row r="28" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="14.25" customHeight="1">
       <c r="A28" s="16">
         <v>3</v>
       </c>
@@ -1834,7 +1878,7 @@
       <c r="Y28" s="16"/>
       <c r="Z28" s="16"/>
     </row>
-    <row r="29" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="14.25" customHeight="1">
       <c r="A29" s="16"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -1866,7 +1910,7 @@
       <c r="Y29" s="16"/>
       <c r="Z29" s="16"/>
     </row>
-    <row r="30" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="14.25" customHeight="1">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -1898,7 +1942,7 @@
       <c r="Y30" s="16"/>
       <c r="Z30" s="16"/>
     </row>
-    <row r="31" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="14.25" customHeight="1">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1930,7 +1974,7 @@
       <c r="Y31" s="16"/>
       <c r="Z31" s="16"/>
     </row>
-    <row r="32" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="14.25" customHeight="1">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1962,7 +2006,7 @@
       <c r="Y32" s="16"/>
       <c r="Z32" s="16"/>
     </row>
-    <row r="33" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" ht="14.25" customHeight="1">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -1994,7 +2038,7 @@
       <c r="Y33" s="16"/>
       <c r="Z33" s="16"/>
     </row>
-    <row r="34" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" ht="14.25" customHeight="1">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -2026,7 +2070,7 @@
       <c r="Y34" s="16"/>
       <c r="Z34" s="16"/>
     </row>
-    <row r="35" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" ht="14.25" customHeight="1">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -2056,7 +2100,7 @@
       <c r="Y35" s="16"/>
       <c r="Z35" s="16"/>
     </row>
-    <row r="36" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" ht="14.25" customHeight="1">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -2086,7 +2130,7 @@
       <c r="Y36" s="16"/>
       <c r="Z36" s="16"/>
     </row>
-    <row r="37" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" ht="14.25" customHeight="1">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -2114,7 +2158,7 @@
       <c r="Y37" s="16"/>
       <c r="Z37" s="16"/>
     </row>
-    <row r="38" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" ht="14.25" customHeight="1">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -2146,7 +2190,7 @@
       <c r="Y38" s="16"/>
       <c r="Z38" s="16"/>
     </row>
-    <row r="39" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" ht="14.25" customHeight="1">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -2174,7 +2218,7 @@
       <c r="Y39" s="16"/>
       <c r="Z39" s="16"/>
     </row>
-    <row r="40" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" ht="14.25" customHeight="1">
       <c r="A40" s="24"/>
       <c r="B40" s="24"/>
       <c r="C40" s="24"/>
@@ -2202,7 +2246,7 @@
       <c r="Y40" s="24"/>
       <c r="Z40" s="24"/>
     </row>
-    <row r="41" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" ht="14.25" customHeight="1">
       <c r="A41" s="24">
         <v>4</v>
       </c>
@@ -2242,7 +2286,7 @@
       <c r="Y41" s="24"/>
       <c r="Z41" s="24"/>
     </row>
-    <row r="42" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" ht="14.25" customHeight="1">
       <c r="A42" s="24"/>
       <c r="B42" s="24"/>
       <c r="C42" s="24"/>
@@ -2272,7 +2316,7 @@
       <c r="Y42" s="24"/>
       <c r="Z42" s="24"/>
     </row>
-    <row r="43" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" ht="14.25" customHeight="1">
       <c r="A43" s="24"/>
       <c r="B43" s="24"/>
       <c r="C43" s="24"/>
@@ -2302,7 +2346,7 @@
       <c r="Y43" s="24"/>
       <c r="Z43" s="24"/>
     </row>
-    <row r="44" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" ht="14.25" customHeight="1">
       <c r="A44" s="24"/>
       <c r="B44" s="24"/>
       <c r="C44" s="24"/>
@@ -2332,7 +2376,7 @@
       <c r="Y44" s="24"/>
       <c r="Z44" s="24"/>
     </row>
-    <row r="45" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" ht="14.25" customHeight="1">
       <c r="A45" s="24"/>
       <c r="B45" s="24"/>
       <c r="C45" s="24"/>
@@ -2362,7 +2406,7 @@
       <c r="Y45" s="24"/>
       <c r="Z45" s="24"/>
     </row>
-    <row r="46" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" ht="14.25" customHeight="1">
       <c r="A46" s="24"/>
       <c r="B46" s="24"/>
       <c r="C46" s="24"/>
@@ -2392,7 +2436,7 @@
       <c r="Y46" s="24"/>
       <c r="Z46" s="24"/>
     </row>
-    <row r="47" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" ht="14.25" customHeight="1">
       <c r="A47" s="24"/>
       <c r="B47" s="24"/>
       <c r="C47" s="24"/>
@@ -2422,7 +2466,7 @@
       <c r="Y47" s="24"/>
       <c r="Z47" s="24"/>
     </row>
-    <row r="48" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" ht="14.25" customHeight="1">
       <c r="A48" s="24"/>
       <c r="B48" s="24"/>
       <c r="C48" s="24"/>
@@ -2452,7 +2496,7 @@
       <c r="Y48" s="24"/>
       <c r="Z48" s="24"/>
     </row>
-    <row r="49" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" ht="14.25" customHeight="1">
       <c r="A49" s="24"/>
       <c r="B49" s="24"/>
       <c r="C49" s="24"/>
@@ -2480,7 +2524,7 @@
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
     </row>
-    <row r="50" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" ht="14.25" customHeight="1">
       <c r="A50" s="24"/>
       <c r="B50" s="24"/>
       <c r="C50" s="24"/>
@@ -2512,7 +2556,7 @@
       <c r="Y50" s="24"/>
       <c r="Z50" s="24"/>
     </row>
-    <row r="51" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" ht="14.25" customHeight="1">
       <c r="A51" s="24"/>
       <c r="B51" s="24"/>
       <c r="C51" s="24"/>
@@ -2540,7 +2584,7 @@
       <c r="Y51" s="24"/>
       <c r="Z51" s="24"/>
     </row>
-    <row r="52" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" ht="14.25" customHeight="1">
       <c r="A52" s="28"/>
       <c r="B52" s="28"/>
       <c r="C52" s="28"/>
@@ -2568,7 +2612,7 @@
       <c r="Y52" s="28"/>
       <c r="Z52" s="28"/>
     </row>
-    <row r="53" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" ht="14.25" customHeight="1">
       <c r="A53" s="28">
         <v>5</v>
       </c>
@@ -2608,7 +2652,7 @@
       <c r="Y53" s="28"/>
       <c r="Z53" s="28"/>
     </row>
-    <row r="54" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" ht="14.25" customHeight="1">
       <c r="A54" s="28"/>
       <c r="B54" s="28"/>
       <c r="C54" s="28"/>
@@ -2640,7 +2684,7 @@
       <c r="Y54" s="28"/>
       <c r="Z54" s="28"/>
     </row>
-    <row r="55" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" ht="14.25" customHeight="1">
       <c r="A55" s="28"/>
       <c r="B55" s="28"/>
       <c r="C55" s="28"/>
@@ -2668,7 +2712,7 @@
       <c r="Y55" s="28"/>
       <c r="Z55" s="28"/>
     </row>
-    <row r="56" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" ht="14.25" customHeight="1">
       <c r="A56" s="28"/>
       <c r="B56" s="28"/>
       <c r="C56" s="28"/>
@@ -2696,7 +2740,7 @@
       <c r="Y56" s="28"/>
       <c r="Z56" s="28"/>
     </row>
-    <row r="57" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" ht="14.25" customHeight="1">
       <c r="A57" s="28"/>
       <c r="B57" s="28"/>
       <c r="C57" s="28"/>
@@ -2724,7 +2768,7 @@
       <c r="Y57" s="28"/>
       <c r="Z57" s="28"/>
     </row>
-    <row r="58" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" ht="14.25" customHeight="1">
       <c r="A58" s="28"/>
       <c r="B58" s="28"/>
       <c r="C58" s="28"/>
@@ -2752,7 +2796,7 @@
       <c r="Y58" s="28"/>
       <c r="Z58" s="28"/>
     </row>
-    <row r="59" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" ht="14.25" customHeight="1">
       <c r="A59" s="29">
         <v>6</v>
       </c>
@@ -2796,7 +2840,7 @@
       <c r="Y59" s="29"/>
       <c r="Z59" s="29"/>
     </row>
-    <row r="60" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" ht="14.25" customHeight="1">
       <c r="A60" s="29"/>
       <c r="B60" s="29"/>
       <c r="C60" s="29"/>
@@ -2826,7 +2870,7 @@
       <c r="Y60" s="29"/>
       <c r="Z60" s="29"/>
     </row>
-    <row r="61" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" ht="14.25" customHeight="1">
       <c r="A61" s="29"/>
       <c r="B61" s="29"/>
       <c r="C61" s="29"/>
@@ -2856,7 +2900,7 @@
       <c r="Y61" s="29"/>
       <c r="Z61" s="29"/>
     </row>
-    <row r="62" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" ht="14.25" customHeight="1">
       <c r="A62" s="29"/>
       <c r="B62" s="29"/>
       <c r="C62" s="29"/>
@@ -2886,7 +2930,7 @@
       <c r="Y62" s="29"/>
       <c r="Z62" s="29"/>
     </row>
-    <row r="63" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" ht="14.25" customHeight="1">
       <c r="A63" s="29"/>
       <c r="B63" s="29"/>
       <c r="C63" s="29"/>
@@ -2920,7 +2964,7 @@
       <c r="Y63" s="29"/>
       <c r="Z63" s="29"/>
     </row>
-    <row r="64" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" ht="14.25" customHeight="1">
       <c r="A64" s="29"/>
       <c r="B64" s="29"/>
       <c r="C64" s="29"/>
@@ -2952,7 +2996,7 @@
       <c r="Y64" s="29"/>
       <c r="Z64" s="29"/>
     </row>
-    <row r="65" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" ht="14.25" customHeight="1">
       <c r="A65" s="32"/>
       <c r="B65" s="32"/>
       <c r="C65" s="32"/>
@@ -2980,7 +3024,7 @@
       <c r="Y65" s="32"/>
       <c r="Z65" s="32"/>
     </row>
-    <row r="66" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" ht="14.25" customHeight="1">
       <c r="A66" s="32">
         <v>7</v>
       </c>
@@ -2990,7 +3034,7 @@
       <c r="C66" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="D66" s="32" t="s">
+      <c r="D66" s="52" t="s">
         <v>11</v>
       </c>
       <c r="E66" s="32"/>
@@ -3020,7 +3064,7 @@
       <c r="Y66" s="32"/>
       <c r="Z66" s="32"/>
     </row>
-    <row r="67" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" ht="14.25" customHeight="1">
       <c r="A67" s="32"/>
       <c r="B67" s="32"/>
       <c r="C67" s="32"/>
@@ -3050,7 +3094,7 @@
       <c r="Y67" s="32"/>
       <c r="Z67" s="32"/>
     </row>
-    <row r="68" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" ht="14.25" customHeight="1">
       <c r="A68" s="32"/>
       <c r="B68" s="32"/>
       <c r="C68" s="32"/>
@@ -3080,7 +3124,7 @@
       <c r="Y68" s="32"/>
       <c r="Z68" s="32"/>
     </row>
-    <row r="69" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" ht="14.25" customHeight="1">
       <c r="A69" s="32"/>
       <c r="B69" s="32"/>
       <c r="C69" s="32"/>
@@ -3110,7 +3154,7 @@
       <c r="Y69" s="32"/>
       <c r="Z69" s="32"/>
     </row>
-    <row r="70" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" ht="14.25" customHeight="1">
       <c r="A70" s="32"/>
       <c r="B70" s="32"/>
       <c r="C70" s="32"/>
@@ -3140,7 +3184,7 @@
       <c r="Y70" s="32"/>
       <c r="Z70" s="32"/>
     </row>
-    <row r="71" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" ht="14.25" customHeight="1">
       <c r="A71" s="32"/>
       <c r="B71" s="32"/>
       <c r="C71" s="32"/>
@@ -3170,7 +3214,7 @@
       <c r="Y71" s="32"/>
       <c r="Z71" s="32"/>
     </row>
-    <row r="72" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" ht="14.25" customHeight="1">
       <c r="A72" s="32"/>
       <c r="B72" s="32"/>
       <c r="C72" s="32"/>
@@ -3198,7 +3242,7 @@
       <c r="Y72" s="32"/>
       <c r="Z72" s="32"/>
     </row>
-    <row r="73" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" ht="14.25" customHeight="1">
       <c r="A73" s="32"/>
       <c r="B73" s="32"/>
       <c r="C73" s="32"/>
@@ -3230,733 +3274,789 @@
       <c r="Y73" s="32"/>
       <c r="Z73" s="32"/>
     </row>
-    <row r="74" spans="1:26" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="1:26" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" s="41" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A74" s="41">
+        <v>8</v>
+      </c>
+      <c r="C74" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="D74" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F74" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="G74" s="53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" s="41" customFormat="1" ht="14.25" customHeight="1">
       <c r="F75" s="42"/>
       <c r="G75" s="42"/>
     </row>
-    <row r="76" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="77" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="78" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="79" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="80" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A80">
+        <v>9</v>
+      </c>
+      <c r="C80" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="D80" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="G80" s="54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="82" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="83" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="84" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A84">
+        <v>10</v>
+      </c>
+      <c r="C84" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="D84" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G84" s="54" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="14.25" customHeight="1">
+      <c r="G85" s="54" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="14.25" customHeight="1">
+      <c r="G86" s="54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="88" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="89" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="90" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="91" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="92" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="93" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="94" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="95" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="96" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="101" ht="14.25" customHeight="1"/>
+    <row r="102" ht="14.25" customHeight="1"/>
+    <row r="103" ht="14.25" customHeight="1"/>
+    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="105" ht="14.25" customHeight="1"/>
+    <row r="106" ht="14.25" customHeight="1"/>
+    <row r="107" ht="14.25" customHeight="1"/>
+    <row r="108" ht="14.25" customHeight="1"/>
+    <row r="109" ht="14.25" customHeight="1"/>
+    <row r="110" ht="14.25" customHeight="1"/>
+    <row r="111" ht="14.25" customHeight="1"/>
+    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="113" ht="14.25" customHeight="1"/>
+    <row r="114" ht="14.25" customHeight="1"/>
+    <row r="115" ht="14.25" customHeight="1"/>
+    <row r="116" ht="14.25" customHeight="1"/>
+    <row r="117" ht="14.25" customHeight="1"/>
+    <row r="118" ht="14.25" customHeight="1"/>
+    <row r="119" ht="14.25" customHeight="1"/>
+    <row r="120" ht="14.25" customHeight="1"/>
+    <row r="121" ht="14.25" customHeight="1"/>
+    <row r="122" ht="14.25" customHeight="1"/>
+    <row r="123" ht="14.25" customHeight="1"/>
+    <row r="124" ht="14.25" customHeight="1"/>
+    <row r="125" ht="14.25" customHeight="1"/>
+    <row r="126" ht="14.25" customHeight="1"/>
+    <row r="127" ht="14.25" customHeight="1"/>
+    <row r="128" ht="14.25" customHeight="1"/>
+    <row r="129" ht="14.25" customHeight="1"/>
+    <row r="130" ht="14.25" customHeight="1"/>
+    <row r="131" ht="14.25" customHeight="1"/>
+    <row r="132" ht="14.25" customHeight="1"/>
+    <row r="133" ht="14.25" customHeight="1"/>
+    <row r="134" ht="14.25" customHeight="1"/>
+    <row r="135" ht="14.25" customHeight="1"/>
+    <row r="136" ht="14.25" customHeight="1"/>
+    <row r="137" ht="14.25" customHeight="1"/>
+    <row r="138" ht="14.25" customHeight="1"/>
+    <row r="139" ht="14.25" customHeight="1"/>
+    <row r="140" ht="14.25" customHeight="1"/>
+    <row r="141" ht="14.25" customHeight="1"/>
+    <row r="142" ht="14.25" customHeight="1"/>
+    <row r="143" ht="14.25" customHeight="1"/>
+    <row r="144" ht="14.25" customHeight="1"/>
+    <row r="145" ht="14.25" customHeight="1"/>
+    <row r="146" ht="14.25" customHeight="1"/>
+    <row r="147" ht="14.25" customHeight="1"/>
+    <row r="148" ht="14.25" customHeight="1"/>
+    <row r="149" ht="14.25" customHeight="1"/>
+    <row r="150" ht="14.25" customHeight="1"/>
+    <row r="151" ht="14.25" customHeight="1"/>
+    <row r="152" ht="14.25" customHeight="1"/>
+    <row r="153" ht="14.25" customHeight="1"/>
+    <row r="154" ht="14.25" customHeight="1"/>
+    <row r="155" ht="14.25" customHeight="1"/>
+    <row r="156" ht="14.25" customHeight="1"/>
+    <row r="157" ht="14.25" customHeight="1"/>
+    <row r="158" ht="14.25" customHeight="1"/>
+    <row r="159" ht="14.25" customHeight="1"/>
+    <row r="160" ht="14.25" customHeight="1"/>
+    <row r="161" ht="14.25" customHeight="1"/>
+    <row r="162" ht="14.25" customHeight="1"/>
+    <row r="163" ht="14.25" customHeight="1"/>
+    <row r="164" ht="14.25" customHeight="1"/>
+    <row r="165" ht="14.25" customHeight="1"/>
+    <row r="166" ht="14.25" customHeight="1"/>
+    <row r="167" ht="14.25" customHeight="1"/>
+    <row r="168" ht="14.25" customHeight="1"/>
+    <row r="169" ht="14.25" customHeight="1"/>
+    <row r="170" ht="14.25" customHeight="1"/>
+    <row r="171" ht="14.25" customHeight="1"/>
+    <row r="172" ht="14.25" customHeight="1"/>
+    <row r="173" ht="14.25" customHeight="1"/>
+    <row r="174" ht="14.25" customHeight="1"/>
+    <row r="175" ht="14.25" customHeight="1"/>
+    <row r="176" ht="14.25" customHeight="1"/>
+    <row r="177" ht="14.25" customHeight="1"/>
+    <row r="178" ht="14.25" customHeight="1"/>
+    <row r="179" ht="14.25" customHeight="1"/>
+    <row r="180" ht="14.25" customHeight="1"/>
+    <row r="181" ht="14.25" customHeight="1"/>
+    <row r="182" ht="14.25" customHeight="1"/>
+    <row r="183" ht="14.25" customHeight="1"/>
+    <row r="184" ht="14.25" customHeight="1"/>
+    <row r="185" ht="14.25" customHeight="1"/>
+    <row r="186" ht="14.25" customHeight="1"/>
+    <row r="187" ht="14.25" customHeight="1"/>
+    <row r="188" ht="14.25" customHeight="1"/>
+    <row r="189" ht="14.25" customHeight="1"/>
+    <row r="190" ht="14.25" customHeight="1"/>
+    <row r="191" ht="14.25" customHeight="1"/>
+    <row r="192" ht="14.25" customHeight="1"/>
+    <row r="193" ht="14.25" customHeight="1"/>
+    <row r="194" ht="14.25" customHeight="1"/>
+    <row r="195" ht="14.25" customHeight="1"/>
+    <row r="196" ht="14.25" customHeight="1"/>
+    <row r="197" ht="14.25" customHeight="1"/>
+    <row r="198" ht="14.25" customHeight="1"/>
+    <row r="199" ht="14.25" customHeight="1"/>
+    <row r="200" ht="14.25" customHeight="1"/>
+    <row r="201" ht="14.25" customHeight="1"/>
+    <row r="202" ht="14.25" customHeight="1"/>
+    <row r="203" ht="14.25" customHeight="1"/>
+    <row r="204" ht="14.25" customHeight="1"/>
+    <row r="205" ht="14.25" customHeight="1"/>
+    <row r="206" ht="14.25" customHeight="1"/>
+    <row r="207" ht="14.25" customHeight="1"/>
+    <row r="208" ht="14.25" customHeight="1"/>
+    <row r="209" ht="14.25" customHeight="1"/>
+    <row r="210" ht="14.25" customHeight="1"/>
+    <row r="211" ht="14.25" customHeight="1"/>
+    <row r="212" ht="14.25" customHeight="1"/>
+    <row r="213" ht="14.25" customHeight="1"/>
+    <row r="214" ht="14.25" customHeight="1"/>
+    <row r="215" ht="14.25" customHeight="1"/>
+    <row r="216" ht="14.25" customHeight="1"/>
+    <row r="217" ht="14.25" customHeight="1"/>
+    <row r="218" ht="14.25" customHeight="1"/>
+    <row r="219" ht="14.25" customHeight="1"/>
+    <row r="220" ht="14.25" customHeight="1"/>
+    <row r="221" ht="14.25" customHeight="1"/>
+    <row r="222" ht="14.25" customHeight="1"/>
+    <row r="223" ht="14.25" customHeight="1"/>
+    <row r="224" ht="14.25" customHeight="1"/>
+    <row r="225" ht="14.25" customHeight="1"/>
+    <row r="226" ht="14.25" customHeight="1"/>
+    <row r="227" ht="14.25" customHeight="1"/>
+    <row r="228" ht="14.25" customHeight="1"/>
+    <row r="229" ht="14.25" customHeight="1"/>
+    <row r="230" ht="14.25" customHeight="1"/>
+    <row r="231" ht="14.25" customHeight="1"/>
+    <row r="232" ht="14.25" customHeight="1"/>
+    <row r="233" ht="14.25" customHeight="1"/>
+    <row r="234" ht="14.25" customHeight="1"/>
+    <row r="235" ht="14.25" customHeight="1"/>
+    <row r="236" ht="14.25" customHeight="1"/>
+    <row r="237" ht="14.25" customHeight="1"/>
+    <row r="238" ht="14.25" customHeight="1"/>
+    <row r="239" ht="14.25" customHeight="1"/>
+    <row r="240" ht="14.25" customHeight="1"/>
+    <row r="241" ht="14.25" customHeight="1"/>
+    <row r="242" ht="14.25" customHeight="1"/>
+    <row r="243" ht="14.25" customHeight="1"/>
+    <row r="244" ht="14.25" customHeight="1"/>
+    <row r="245" ht="14.25" customHeight="1"/>
+    <row r="246" ht="14.25" customHeight="1"/>
+    <row r="247" ht="14.25" customHeight="1"/>
+    <row r="248" ht="14.25" customHeight="1"/>
+    <row r="249" ht="14.25" customHeight="1"/>
+    <row r="250" ht="14.25" customHeight="1"/>
+    <row r="251" ht="14.25" customHeight="1"/>
+    <row r="252" ht="14.25" customHeight="1"/>
+    <row r="253" ht="14.25" customHeight="1"/>
+    <row r="254" ht="14.25" customHeight="1"/>
+    <row r="255" ht="14.25" customHeight="1"/>
+    <row r="256" ht="14.25" customHeight="1"/>
+    <row r="257" ht="14.25" customHeight="1"/>
+    <row r="258" ht="14.25" customHeight="1"/>
+    <row r="259" ht="14.25" customHeight="1"/>
+    <row r="260" ht="14.25" customHeight="1"/>
+    <row r="261" ht="14.25" customHeight="1"/>
+    <row r="262" ht="14.25" customHeight="1"/>
+    <row r="263" ht="14.25" customHeight="1"/>
+    <row r="264" ht="14.25" customHeight="1"/>
+    <row r="265" ht="14.25" customHeight="1"/>
+    <row r="266" ht="14.25" customHeight="1"/>
+    <row r="267" ht="14.25" customHeight="1"/>
+    <row r="268" ht="14.25" customHeight="1"/>
+    <row r="269" ht="14.25" customHeight="1"/>
+    <row r="270" ht="14.25" customHeight="1"/>
+    <row r="271" ht="14.25" customHeight="1"/>
+    <row r="272" ht="14.25" customHeight="1"/>
+    <row r="273" ht="14.25" customHeight="1"/>
+    <row r="274" ht="14.25" customHeight="1"/>
+    <row r="275" ht="14.25" customHeight="1"/>
+    <row r="276" ht="14.25" customHeight="1"/>
+    <row r="277" ht="14.25" customHeight="1"/>
+    <row r="278" ht="14.25" customHeight="1"/>
+    <row r="279" ht="14.25" customHeight="1"/>
+    <row r="280" ht="14.25" customHeight="1"/>
+    <row r="281" ht="14.25" customHeight="1"/>
+    <row r="282" ht="14.25" customHeight="1"/>
+    <row r="283" ht="14.25" customHeight="1"/>
+    <row r="284" ht="14.25" customHeight="1"/>
+    <row r="285" ht="14.25" customHeight="1"/>
+    <row r="286" ht="14.25" customHeight="1"/>
+    <row r="287" ht="14.25" customHeight="1"/>
+    <row r="288" ht="14.25" customHeight="1"/>
+    <row r="289" ht="14.25" customHeight="1"/>
+    <row r="290" ht="14.25" customHeight="1"/>
+    <row r="291" ht="14.25" customHeight="1"/>
+    <row r="292" ht="14.25" customHeight="1"/>
+    <row r="293" ht="14.25" customHeight="1"/>
+    <row r="294" ht="14.25" customHeight="1"/>
+    <row r="295" ht="14.25" customHeight="1"/>
+    <row r="296" ht="14.25" customHeight="1"/>
+    <row r="297" ht="14.25" customHeight="1"/>
+    <row r="298" ht="14.25" customHeight="1"/>
+    <row r="299" ht="14.25" customHeight="1"/>
+    <row r="300" ht="14.25" customHeight="1"/>
+    <row r="301" ht="14.25" customHeight="1"/>
+    <row r="302" ht="14.25" customHeight="1"/>
+    <row r="303" ht="14.25" customHeight="1"/>
+    <row r="304" ht="14.25" customHeight="1"/>
+    <row r="305" ht="14.25" customHeight="1"/>
+    <row r="306" ht="14.25" customHeight="1"/>
+    <row r="307" ht="14.25" customHeight="1"/>
+    <row r="308" ht="14.25" customHeight="1"/>
+    <row r="309" ht="14.25" customHeight="1"/>
+    <row r="310" ht="14.25" customHeight="1"/>
+    <row r="311" ht="14.25" customHeight="1"/>
+    <row r="312" ht="14.25" customHeight="1"/>
+    <row r="313" ht="14.25" customHeight="1"/>
+    <row r="314" ht="14.25" customHeight="1"/>
+    <row r="315" ht="14.25" customHeight="1"/>
+    <row r="316" ht="14.25" customHeight="1"/>
+    <row r="317" ht="14.25" customHeight="1"/>
+    <row r="318" ht="14.25" customHeight="1"/>
+    <row r="319" ht="14.25" customHeight="1"/>
+    <row r="320" ht="14.25" customHeight="1"/>
+    <row r="321" ht="14.25" customHeight="1"/>
+    <row r="322" ht="14.25" customHeight="1"/>
+    <row r="323" ht="14.25" customHeight="1"/>
+    <row r="324" ht="14.25" customHeight="1"/>
+    <row r="325" ht="14.25" customHeight="1"/>
+    <row r="326" ht="14.25" customHeight="1"/>
+    <row r="327" ht="14.25" customHeight="1"/>
+    <row r="328" ht="14.25" customHeight="1"/>
+    <row r="329" ht="14.25" customHeight="1"/>
+    <row r="330" ht="14.25" customHeight="1"/>
+    <row r="331" ht="14.25" customHeight="1"/>
+    <row r="332" ht="14.25" customHeight="1"/>
+    <row r="333" ht="14.25" customHeight="1"/>
+    <row r="334" ht="14.25" customHeight="1"/>
+    <row r="335" ht="14.25" customHeight="1"/>
+    <row r="336" ht="14.25" customHeight="1"/>
+    <row r="337" ht="14.25" customHeight="1"/>
+    <row r="338" ht="14.25" customHeight="1"/>
+    <row r="339" ht="14.25" customHeight="1"/>
+    <row r="340" ht="14.25" customHeight="1"/>
+    <row r="341" ht="14.25" customHeight="1"/>
+    <row r="342" ht="14.25" customHeight="1"/>
+    <row r="343" ht="14.25" customHeight="1"/>
+    <row r="344" ht="14.25" customHeight="1"/>
+    <row r="345" ht="14.25" customHeight="1"/>
+    <row r="346" ht="14.25" customHeight="1"/>
+    <row r="347" ht="14.25" customHeight="1"/>
+    <row r="348" ht="14.25" customHeight="1"/>
+    <row r="349" ht="14.25" customHeight="1"/>
+    <row r="350" ht="14.25" customHeight="1"/>
+    <row r="351" ht="14.25" customHeight="1"/>
+    <row r="352" ht="14.25" customHeight="1"/>
+    <row r="353" ht="14.25" customHeight="1"/>
+    <row r="354" ht="14.25" customHeight="1"/>
+    <row r="355" ht="14.25" customHeight="1"/>
+    <row r="356" ht="14.25" customHeight="1"/>
+    <row r="357" ht="14.25" customHeight="1"/>
+    <row r="358" ht="14.25" customHeight="1"/>
+    <row r="359" ht="14.25" customHeight="1"/>
+    <row r="360" ht="14.25" customHeight="1"/>
+    <row r="361" ht="14.25" customHeight="1"/>
+    <row r="362" ht="14.25" customHeight="1"/>
+    <row r="363" ht="14.25" customHeight="1"/>
+    <row r="364" ht="14.25" customHeight="1"/>
+    <row r="365" ht="14.25" customHeight="1"/>
+    <row r="366" ht="14.25" customHeight="1"/>
+    <row r="367" ht="14.25" customHeight="1"/>
+    <row r="368" ht="14.25" customHeight="1"/>
+    <row r="369" ht="14.25" customHeight="1"/>
+    <row r="370" ht="14.25" customHeight="1"/>
+    <row r="371" ht="14.25" customHeight="1"/>
+    <row r="372" ht="14.25" customHeight="1"/>
+    <row r="373" ht="14.25" customHeight="1"/>
+    <row r="374" ht="14.25" customHeight="1"/>
+    <row r="375" ht="14.25" customHeight="1"/>
+    <row r="376" ht="14.25" customHeight="1"/>
+    <row r="377" ht="14.25" customHeight="1"/>
+    <row r="378" ht="14.25" customHeight="1"/>
+    <row r="379" ht="14.25" customHeight="1"/>
+    <row r="380" ht="14.25" customHeight="1"/>
+    <row r="381" ht="14.25" customHeight="1"/>
+    <row r="382" ht="14.25" customHeight="1"/>
+    <row r="383" ht="14.25" customHeight="1"/>
+    <row r="384" ht="14.25" customHeight="1"/>
+    <row r="385" ht="14.25" customHeight="1"/>
+    <row r="386" ht="14.25" customHeight="1"/>
+    <row r="387" ht="14.25" customHeight="1"/>
+    <row r="388" ht="14.25" customHeight="1"/>
+    <row r="389" ht="14.25" customHeight="1"/>
+    <row r="390" ht="14.25" customHeight="1"/>
+    <row r="391" ht="14.25" customHeight="1"/>
+    <row r="392" ht="14.25" customHeight="1"/>
+    <row r="393" ht="14.25" customHeight="1"/>
+    <row r="394" ht="14.25" customHeight="1"/>
+    <row r="395" ht="14.25" customHeight="1"/>
+    <row r="396" ht="14.25" customHeight="1"/>
+    <row r="397" ht="14.25" customHeight="1"/>
+    <row r="398" ht="14.25" customHeight="1"/>
+    <row r="399" ht="14.25" customHeight="1"/>
+    <row r="400" ht="14.25" customHeight="1"/>
+    <row r="401" ht="14.25" customHeight="1"/>
+    <row r="402" ht="14.25" customHeight="1"/>
+    <row r="403" ht="14.25" customHeight="1"/>
+    <row r="404" ht="14.25" customHeight="1"/>
+    <row r="405" ht="14.25" customHeight="1"/>
+    <row r="406" ht="14.25" customHeight="1"/>
+    <row r="407" ht="14.25" customHeight="1"/>
+    <row r="408" ht="14.25" customHeight="1"/>
+    <row r="409" ht="14.25" customHeight="1"/>
+    <row r="410" ht="14.25" customHeight="1"/>
+    <row r="411" ht="14.25" customHeight="1"/>
+    <row r="412" ht="14.25" customHeight="1"/>
+    <row r="413" ht="14.25" customHeight="1"/>
+    <row r="414" ht="14.25" customHeight="1"/>
+    <row r="415" ht="14.25" customHeight="1"/>
+    <row r="416" ht="14.25" customHeight="1"/>
+    <row r="417" ht="14.25" customHeight="1"/>
+    <row r="418" ht="14.25" customHeight="1"/>
+    <row r="419" ht="14.25" customHeight="1"/>
+    <row r="420" ht="14.25" customHeight="1"/>
+    <row r="421" ht="14.25" customHeight="1"/>
+    <row r="422" ht="14.25" customHeight="1"/>
+    <row r="423" ht="14.25" customHeight="1"/>
+    <row r="424" ht="14.25" customHeight="1"/>
+    <row r="425" ht="14.25" customHeight="1"/>
+    <row r="426" ht="14.25" customHeight="1"/>
+    <row r="427" ht="14.25" customHeight="1"/>
+    <row r="428" ht="14.25" customHeight="1"/>
+    <row r="429" ht="14.25" customHeight="1"/>
+    <row r="430" ht="14.25" customHeight="1"/>
+    <row r="431" ht="14.25" customHeight="1"/>
+    <row r="432" ht="14.25" customHeight="1"/>
+    <row r="433" ht="14.25" customHeight="1"/>
+    <row r="434" ht="14.25" customHeight="1"/>
+    <row r="435" ht="14.25" customHeight="1"/>
+    <row r="436" ht="14.25" customHeight="1"/>
+    <row r="437" ht="14.25" customHeight="1"/>
+    <row r="438" ht="14.25" customHeight="1"/>
+    <row r="439" ht="14.25" customHeight="1"/>
+    <row r="440" ht="14.25" customHeight="1"/>
+    <row r="441" ht="14.25" customHeight="1"/>
+    <row r="442" ht="14.25" customHeight="1"/>
+    <row r="443" ht="14.25" customHeight="1"/>
+    <row r="444" ht="14.25" customHeight="1"/>
+    <row r="445" ht="14.25" customHeight="1"/>
+    <row r="446" ht="14.25" customHeight="1"/>
+    <row r="447" ht="14.25" customHeight="1"/>
+    <row r="448" ht="14.25" customHeight="1"/>
+    <row r="449" ht="14.25" customHeight="1"/>
+    <row r="450" ht="14.25" customHeight="1"/>
+    <row r="451" ht="14.25" customHeight="1"/>
+    <row r="452" ht="14.25" customHeight="1"/>
+    <row r="453" ht="14.25" customHeight="1"/>
+    <row r="454" ht="14.25" customHeight="1"/>
+    <row r="455" ht="14.25" customHeight="1"/>
+    <row r="456" ht="14.25" customHeight="1"/>
+    <row r="457" ht="14.25" customHeight="1"/>
+    <row r="458" ht="14.25" customHeight="1"/>
+    <row r="459" ht="14.25" customHeight="1"/>
+    <row r="460" ht="14.25" customHeight="1"/>
+    <row r="461" ht="14.25" customHeight="1"/>
+    <row r="462" ht="14.25" customHeight="1"/>
+    <row r="463" ht="14.25" customHeight="1"/>
+    <row r="464" ht="14.25" customHeight="1"/>
+    <row r="465" ht="14.25" customHeight="1"/>
+    <row r="466" ht="14.25" customHeight="1"/>
+    <row r="467" ht="14.25" customHeight="1"/>
+    <row r="468" ht="14.25" customHeight="1"/>
+    <row r="469" ht="14.25" customHeight="1"/>
+    <row r="470" ht="14.25" customHeight="1"/>
+    <row r="471" ht="14.25" customHeight="1"/>
+    <row r="472" ht="14.25" customHeight="1"/>
+    <row r="473" ht="14.25" customHeight="1"/>
+    <row r="474" ht="14.25" customHeight="1"/>
+    <row r="475" ht="14.25" customHeight="1"/>
+    <row r="476" ht="14.25" customHeight="1"/>
+    <row r="477" ht="14.25" customHeight="1"/>
+    <row r="478" ht="14.25" customHeight="1"/>
+    <row r="479" ht="14.25" customHeight="1"/>
+    <row r="480" ht="14.25" customHeight="1"/>
+    <row r="481" ht="14.25" customHeight="1"/>
+    <row r="482" ht="14.25" customHeight="1"/>
+    <row r="483" ht="14.25" customHeight="1"/>
+    <row r="484" ht="14.25" customHeight="1"/>
+    <row r="485" ht="14.25" customHeight="1"/>
+    <row r="486" ht="14.25" customHeight="1"/>
+    <row r="487" ht="14.25" customHeight="1"/>
+    <row r="488" ht="14.25" customHeight="1"/>
+    <row r="489" ht="14.25" customHeight="1"/>
+    <row r="490" ht="14.25" customHeight="1"/>
+    <row r="491" ht="14.25" customHeight="1"/>
+    <row r="492" ht="14.25" customHeight="1"/>
+    <row r="493" ht="14.25" customHeight="1"/>
+    <row r="494" ht="14.25" customHeight="1"/>
+    <row r="495" ht="14.25" customHeight="1"/>
+    <row r="496" ht="14.25" customHeight="1"/>
+    <row r="497" ht="14.25" customHeight="1"/>
+    <row r="498" ht="14.25" customHeight="1"/>
+    <row r="499" ht="14.25" customHeight="1"/>
+    <row r="500" ht="14.25" customHeight="1"/>
+    <row r="501" ht="14.25" customHeight="1"/>
+    <row r="502" ht="14.25" customHeight="1"/>
+    <row r="503" ht="14.25" customHeight="1"/>
+    <row r="504" ht="14.25" customHeight="1"/>
+    <row r="505" ht="14.25" customHeight="1"/>
+    <row r="506" ht="14.25" customHeight="1"/>
+    <row r="507" ht="14.25" customHeight="1"/>
+    <row r="508" ht="14.25" customHeight="1"/>
+    <row r="509" ht="14.25" customHeight="1"/>
+    <row r="510" ht="14.25" customHeight="1"/>
+    <row r="511" ht="14.25" customHeight="1"/>
+    <row r="512" ht="14.25" customHeight="1"/>
+    <row r="513" ht="14.25" customHeight="1"/>
+    <row r="514" ht="14.25" customHeight="1"/>
+    <row r="515" ht="14.25" customHeight="1"/>
+    <row r="516" ht="14.25" customHeight="1"/>
+    <row r="517" ht="14.25" customHeight="1"/>
+    <row r="518" ht="14.25" customHeight="1"/>
+    <row r="519" ht="14.25" customHeight="1"/>
+    <row r="520" ht="14.25" customHeight="1"/>
+    <row r="521" ht="14.25" customHeight="1"/>
+    <row r="522" ht="14.25" customHeight="1"/>
+    <row r="523" ht="14.25" customHeight="1"/>
+    <row r="524" ht="14.25" customHeight="1"/>
+    <row r="525" ht="14.25" customHeight="1"/>
+    <row r="526" ht="14.25" customHeight="1"/>
+    <row r="527" ht="14.25" customHeight="1"/>
+    <row r="528" ht="14.25" customHeight="1"/>
+    <row r="529" ht="14.25" customHeight="1"/>
+    <row r="530" ht="14.25" customHeight="1"/>
+    <row r="531" ht="14.25" customHeight="1"/>
+    <row r="532" ht="14.25" customHeight="1"/>
+    <row r="533" ht="14.25" customHeight="1"/>
+    <row r="534" ht="14.25" customHeight="1"/>
+    <row r="535" ht="14.25" customHeight="1"/>
+    <row r="536" ht="14.25" customHeight="1"/>
+    <row r="537" ht="14.25" customHeight="1"/>
+    <row r="538" ht="14.25" customHeight="1"/>
+    <row r="539" ht="14.25" customHeight="1"/>
+    <row r="540" ht="14.25" customHeight="1"/>
+    <row r="541" ht="14.25" customHeight="1"/>
+    <row r="542" ht="14.25" customHeight="1"/>
+    <row r="543" ht="14.25" customHeight="1"/>
+    <row r="544" ht="14.25" customHeight="1"/>
+    <row r="545" ht="14.25" customHeight="1"/>
+    <row r="546" ht="14.25" customHeight="1"/>
+    <row r="547" ht="14.25" customHeight="1"/>
+    <row r="548" ht="14.25" customHeight="1"/>
+    <row r="549" ht="14.25" customHeight="1"/>
+    <row r="550" ht="14.25" customHeight="1"/>
+    <row r="551" ht="14.25" customHeight="1"/>
+    <row r="552" ht="14.25" customHeight="1"/>
+    <row r="553" ht="14.25" customHeight="1"/>
+    <row r="554" ht="14.25" customHeight="1"/>
+    <row r="555" ht="14.25" customHeight="1"/>
+    <row r="556" ht="14.25" customHeight="1"/>
+    <row r="557" ht="14.25" customHeight="1"/>
+    <row r="558" ht="14.25" customHeight="1"/>
+    <row r="559" ht="14.25" customHeight="1"/>
+    <row r="560" ht="14.25" customHeight="1"/>
+    <row r="561" ht="14.25" customHeight="1"/>
+    <row r="562" ht="14.25" customHeight="1"/>
+    <row r="563" ht="14.25" customHeight="1"/>
+    <row r="564" ht="14.25" customHeight="1"/>
+    <row r="565" ht="14.25" customHeight="1"/>
+    <row r="566" ht="14.25" customHeight="1"/>
+    <row r="567" ht="14.25" customHeight="1"/>
+    <row r="568" ht="14.25" customHeight="1"/>
+    <row r="569" ht="14.25" customHeight="1"/>
+    <row r="570" ht="14.25" customHeight="1"/>
+    <row r="571" ht="14.25" customHeight="1"/>
+    <row r="572" ht="14.25" customHeight="1"/>
+    <row r="573" ht="14.25" customHeight="1"/>
+    <row r="574" ht="14.25" customHeight="1"/>
+    <row r="575" ht="14.25" customHeight="1"/>
+    <row r="576" ht="14.25" customHeight="1"/>
+    <row r="577" ht="14.25" customHeight="1"/>
+    <row r="578" ht="14.25" customHeight="1"/>
+    <row r="579" ht="14.25" customHeight="1"/>
+    <row r="580" ht="14.25" customHeight="1"/>
+    <row r="581" ht="14.25" customHeight="1"/>
+    <row r="582" ht="14.25" customHeight="1"/>
+    <row r="583" ht="14.25" customHeight="1"/>
+    <row r="584" ht="14.25" customHeight="1"/>
+    <row r="585" ht="14.25" customHeight="1"/>
+    <row r="586" ht="14.25" customHeight="1"/>
+    <row r="587" ht="14.25" customHeight="1"/>
+    <row r="588" ht="14.25" customHeight="1"/>
+    <row r="589" ht="14.25" customHeight="1"/>
+    <row r="590" ht="14.25" customHeight="1"/>
+    <row r="591" ht="14.25" customHeight="1"/>
+    <row r="592" ht="14.25" customHeight="1"/>
+    <row r="593" ht="14.25" customHeight="1"/>
+    <row r="594" ht="14.25" customHeight="1"/>
+    <row r="595" ht="14.25" customHeight="1"/>
+    <row r="596" ht="14.25" customHeight="1"/>
+    <row r="597" ht="14.25" customHeight="1"/>
+    <row r="598" ht="14.25" customHeight="1"/>
+    <row r="599" ht="14.25" customHeight="1"/>
+    <row r="600" ht="14.25" customHeight="1"/>
+    <row r="601" ht="14.25" customHeight="1"/>
+    <row r="602" ht="14.25" customHeight="1"/>
+    <row r="603" ht="14.25" customHeight="1"/>
+    <row r="604" ht="14.25" customHeight="1"/>
+    <row r="605" ht="14.25" customHeight="1"/>
+    <row r="606" ht="14.25" customHeight="1"/>
+    <row r="607" ht="14.25" customHeight="1"/>
+    <row r="608" ht="14.25" customHeight="1"/>
+    <row r="609" ht="14.25" customHeight="1"/>
+    <row r="610" ht="14.25" customHeight="1"/>
+    <row r="611" ht="14.25" customHeight="1"/>
+    <row r="612" ht="14.25" customHeight="1"/>
+    <row r="613" ht="14.25" customHeight="1"/>
+    <row r="614" ht="14.25" customHeight="1"/>
+    <row r="615" ht="14.25" customHeight="1"/>
+    <row r="616" ht="14.25" customHeight="1"/>
+    <row r="617" ht="14.25" customHeight="1"/>
+    <row r="618" ht="14.25" customHeight="1"/>
+    <row r="619" ht="14.25" customHeight="1"/>
+    <row r="620" ht="14.25" customHeight="1"/>
+    <row r="621" ht="14.25" customHeight="1"/>
+    <row r="622" ht="14.25" customHeight="1"/>
+    <row r="623" ht="14.25" customHeight="1"/>
+    <row r="624" ht="14.25" customHeight="1"/>
+    <row r="625" ht="14.25" customHeight="1"/>
+    <row r="626" ht="14.25" customHeight="1"/>
+    <row r="627" ht="14.25" customHeight="1"/>
+    <row r="628" ht="14.25" customHeight="1"/>
+    <row r="629" ht="14.25" customHeight="1"/>
+    <row r="630" ht="14.25" customHeight="1"/>
+    <row r="631" ht="14.25" customHeight="1"/>
+    <row r="632" ht="14.25" customHeight="1"/>
+    <row r="633" ht="14.25" customHeight="1"/>
+    <row r="634" ht="14.25" customHeight="1"/>
+    <row r="635" ht="14.25" customHeight="1"/>
+    <row r="636" ht="14.25" customHeight="1"/>
+    <row r="637" ht="14.25" customHeight="1"/>
+    <row r="638" ht="14.25" customHeight="1"/>
+    <row r="639" ht="14.25" customHeight="1"/>
+    <row r="640" ht="14.25" customHeight="1"/>
+    <row r="641" ht="14.25" customHeight="1"/>
+    <row r="642" ht="14.25" customHeight="1"/>
+    <row r="643" ht="14.25" customHeight="1"/>
+    <row r="644" ht="14.25" customHeight="1"/>
+    <row r="645" ht="14.25" customHeight="1"/>
+    <row r="646" ht="14.25" customHeight="1"/>
+    <row r="647" ht="14.25" customHeight="1"/>
+    <row r="648" ht="14.25" customHeight="1"/>
+    <row r="649" ht="14.25" customHeight="1"/>
+    <row r="650" ht="14.25" customHeight="1"/>
+    <row r="651" ht="14.25" customHeight="1"/>
+    <row r="652" ht="14.25" customHeight="1"/>
+    <row r="653" ht="14.25" customHeight="1"/>
+    <row r="654" ht="14.25" customHeight="1"/>
+    <row r="655" ht="14.25" customHeight="1"/>
+    <row r="656" ht="14.25" customHeight="1"/>
+    <row r="657" ht="14.25" customHeight="1"/>
+    <row r="658" ht="14.25" customHeight="1"/>
+    <row r="659" ht="14.25" customHeight="1"/>
+    <row r="660" ht="14.25" customHeight="1"/>
+    <row r="661" ht="14.25" customHeight="1"/>
+    <row r="662" ht="14.25" customHeight="1"/>
+    <row r="663" ht="14.25" customHeight="1"/>
+    <row r="664" ht="14.25" customHeight="1"/>
+    <row r="665" ht="14.25" customHeight="1"/>
+    <row r="666" ht="14.25" customHeight="1"/>
+    <row r="667" ht="14.25" customHeight="1"/>
+    <row r="668" ht="14.25" customHeight="1"/>
+    <row r="669" ht="14.25" customHeight="1"/>
+    <row r="670" ht="14.25" customHeight="1"/>
+    <row r="671" ht="14.25" customHeight="1"/>
+    <row r="672" ht="14.25" customHeight="1"/>
+    <row r="673" ht="14.25" customHeight="1"/>
+    <row r="674" ht="14.25" customHeight="1"/>
+    <row r="675" ht="14.25" customHeight="1"/>
+    <row r="676" ht="14.25" customHeight="1"/>
+    <row r="677" ht="14.25" customHeight="1"/>
+    <row r="678" ht="14.25" customHeight="1"/>
+    <row r="679" ht="14.25" customHeight="1"/>
+    <row r="680" ht="14.25" customHeight="1"/>
+    <row r="681" ht="14.25" customHeight="1"/>
+    <row r="682" ht="14.25" customHeight="1"/>
+    <row r="683" ht="14.25" customHeight="1"/>
+    <row r="684" ht="14.25" customHeight="1"/>
+    <row r="685" ht="14.25" customHeight="1"/>
+    <row r="686" ht="14.25" customHeight="1"/>
+    <row r="687" ht="14.25" customHeight="1"/>
+    <row r="688" ht="14.25" customHeight="1"/>
+    <row r="689" ht="14.25" customHeight="1"/>
+    <row r="690" ht="14.25" customHeight="1"/>
+    <row r="691" ht="14.25" customHeight="1"/>
+    <row r="692" ht="14.25" customHeight="1"/>
+    <row r="693" ht="14.25" customHeight="1"/>
+    <row r="694" ht="14.25" customHeight="1"/>
+    <row r="695" ht="14.25" customHeight="1"/>
+    <row r="696" ht="14.25" customHeight="1"/>
+    <row r="697" ht="14.25" customHeight="1"/>
+    <row r="698" ht="14.25" customHeight="1"/>
+    <row r="699" ht="14.25" customHeight="1"/>
+    <row r="700" ht="14.25" customHeight="1"/>
+    <row r="701" ht="14.25" customHeight="1"/>
+    <row r="702" ht="14.25" customHeight="1"/>
+    <row r="703" ht="14.25" customHeight="1"/>
+    <row r="704" ht="14.25" customHeight="1"/>
+    <row r="705" ht="14.25" customHeight="1"/>
+    <row r="706" ht="14.25" customHeight="1"/>
+    <row r="707" ht="14.25" customHeight="1"/>
+    <row r="708" ht="14.25" customHeight="1"/>
+    <row r="709" ht="14.25" customHeight="1"/>
+    <row r="710" ht="14.25" customHeight="1"/>
+    <row r="711" ht="14.25" customHeight="1"/>
+    <row r="712" ht="14.25" customHeight="1"/>
+    <row r="713" ht="14.25" customHeight="1"/>
+    <row r="714" ht="14.25" customHeight="1"/>
+    <row r="715" ht="14.25" customHeight="1"/>
+    <row r="716" ht="14.25" customHeight="1"/>
+    <row r="717" ht="14.25" customHeight="1"/>
+    <row r="718" ht="14.25" customHeight="1"/>
+    <row r="719" ht="14.25" customHeight="1"/>
+    <row r="720" ht="14.25" customHeight="1"/>
+    <row r="721" ht="14.25" customHeight="1"/>
+    <row r="722" ht="14.25" customHeight="1"/>
+    <row r="723" ht="14.25" customHeight="1"/>
+    <row r="724" ht="14.25" customHeight="1"/>
+    <row r="725" ht="14.25" customHeight="1"/>
+    <row r="726" ht="14.25" customHeight="1"/>
+    <row r="727" ht="14.25" customHeight="1"/>
+    <row r="728" ht="14.25" customHeight="1"/>
+    <row r="729" ht="14.25" customHeight="1"/>
+    <row r="730" ht="14.25" customHeight="1"/>
+    <row r="731" ht="14.25" customHeight="1"/>
+    <row r="732" ht="14.25" customHeight="1"/>
+    <row r="733" ht="14.25" customHeight="1"/>
+    <row r="734" ht="14.25" customHeight="1"/>
+    <row r="735" ht="14.25" customHeight="1"/>
+    <row r="736" ht="14.25" customHeight="1"/>
+    <row r="737" ht="14.25" customHeight="1"/>
+    <row r="738" ht="14.25" customHeight="1"/>
+    <row r="739" ht="14.25" customHeight="1"/>
+    <row r="740" ht="14.25" customHeight="1"/>
+    <row r="741" ht="14.25" customHeight="1"/>
+    <row r="742" ht="14.25" customHeight="1"/>
+    <row r="743" ht="14.25" customHeight="1"/>
+    <row r="744" ht="14.25" customHeight="1"/>
+    <row r="745" ht="14.25" customHeight="1"/>
+    <row r="746" ht="14.25" customHeight="1"/>
+    <row r="747" ht="14.25" customHeight="1"/>
+    <row r="748" ht="14.25" customHeight="1"/>
+    <row r="749" ht="14.25" customHeight="1"/>
+    <row r="750" ht="14.25" customHeight="1"/>
+    <row r="751" ht="14.25" customHeight="1"/>
+    <row r="752" ht="14.25" customHeight="1"/>
+    <row r="753" ht="14.25" customHeight="1"/>
+    <row r="754" ht="14.25" customHeight="1"/>
+    <row r="755" ht="14.25" customHeight="1"/>
+    <row r="756" ht="14.25" customHeight="1"/>
+    <row r="757" ht="14.25" customHeight="1"/>
+    <row r="758" ht="14.25" customHeight="1"/>
+    <row r="759" ht="14.25" customHeight="1"/>
+    <row r="760" ht="14.25" customHeight="1"/>
+    <row r="761" ht="14.25" customHeight="1"/>
+    <row r="762" ht="14.25" customHeight="1"/>
+    <row r="763" ht="14.25" customHeight="1"/>
+    <row r="764" ht="14.25" customHeight="1"/>
+    <row r="765" ht="14.25" customHeight="1"/>
+    <row r="766" ht="14.25" customHeight="1"/>
+    <row r="767" ht="14.25" customHeight="1"/>
+    <row r="768" ht="14.25" customHeight="1"/>
+    <row r="769" ht="14.25" customHeight="1"/>
+    <row r="770" ht="14.25" customHeight="1"/>
+    <row r="771" ht="14.25" customHeight="1"/>
+    <row r="772" ht="14.25" customHeight="1"/>
+    <row r="773" ht="14.25" customHeight="1"/>
+    <row r="774" ht="14.25" customHeight="1"/>
+    <row r="775" ht="14.25" customHeight="1"/>
+    <row r="776" ht="14.25" customHeight="1"/>
+    <row r="777" ht="14.25" customHeight="1"/>
+    <row r="778" ht="14.25" customHeight="1"/>
+    <row r="779" ht="14.25" customHeight="1"/>
+    <row r="780" ht="14.25" customHeight="1"/>
+    <row r="781" ht="14.25" customHeight="1"/>
+    <row r="782" ht="14.25" customHeight="1"/>
+    <row r="783" ht="14.25" customHeight="1"/>
+    <row r="784" ht="14.25" customHeight="1"/>
+    <row r="785" ht="14.25" customHeight="1"/>
+    <row r="786" ht="14.25" customHeight="1"/>
+    <row r="787" ht="14.25" customHeight="1"/>
+    <row r="788" ht="14.25" customHeight="1"/>
+    <row r="789" ht="14.25" customHeight="1"/>
+    <row r="790" ht="14.25" customHeight="1"/>
+    <row r="791" ht="14.25" customHeight="1"/>
+    <row r="792" ht="14.25" customHeight="1"/>
+    <row r="793" ht="14.25" customHeight="1"/>
+    <row r="794" ht="14.25" customHeight="1"/>
+    <row r="795" ht="14.25" customHeight="1"/>
+    <row r="796" ht="14.25" customHeight="1"/>
+    <row r="797" ht="14.25" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C66" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -3978,16 +4078,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="10" width="8.6640625" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="12" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" customWidth="1"/>
+    <col min="2" max="10" width="8.6328125" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" customWidth="1"/>
+    <col min="12" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:17" ht="14.25" customHeight="1">
       <c r="B2" s="35" t="s">
         <v>58</v>
       </c>
@@ -4001,7 +4101,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="14.25" customHeight="1">
       <c r="B3" s="35" t="s">
         <v>62</v>
       </c>
@@ -4018,7 +4118,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="14.25" customHeight="1">
       <c r="A4" s="36" t="s">
         <v>67</v>
       </c>
@@ -4029,7 +4129,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="14.25" customHeight="1">
       <c r="A5" s="35" t="s">
         <v>70</v>
       </c>
@@ -4040,7 +4140,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="14.25" customHeight="1">
       <c r="A6" s="35" t="s">
         <v>73</v>
       </c>
@@ -4054,7 +4154,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="14.25" customHeight="1">
       <c r="B7" s="35" t="s">
         <v>77</v>
       </c>
@@ -4062,7 +4162,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>79</v>
       </c>
@@ -4070,12 +4170,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="14.25" customHeight="1">
       <c r="A9" s="35" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="14.25" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>82</v>
       </c>
@@ -4095,7 +4195,7 @@
       <c r="P10" s="38"/>
       <c r="Q10" s="38"/>
     </row>
-    <row r="11" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="14.25" customHeight="1">
       <c r="A11" s="35" t="s">
         <v>71</v>
       </c>
@@ -4121,7 +4221,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="14.25" customHeight="1">
       <c r="D12" s="35" t="s">
         <v>89</v>
       </c>
@@ -4144,7 +4244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="14.25" customHeight="1">
       <c r="A13" s="35" t="s">
         <v>86</v>
       </c>
@@ -4160,29 +4260,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="14.25" customHeight="1">
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
       <c r="O14" s="38"/>
       <c r="P14" s="38"/>
       <c r="Q14" s="38"/>
     </row>
-    <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="14.25" customHeight="1">
       <c r="L15" s="38"/>
       <c r="M15" s="38"/>
       <c r="O15" s="38"/>
       <c r="P15" s="38"/>
       <c r="Q15" s="38"/>
     </row>
-    <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="14.25" customHeight="1">
       <c r="L16" s="38"/>
       <c r="M16" s="38"/>
       <c r="O16" s="38"/>
       <c r="P16" s="38"/>
       <c r="Q16" s="38"/>
     </row>
-    <row r="17" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:19" ht="14.25" customHeight="1">
       <c r="A18" s="35" t="s">
         <v>93</v>
       </c>
@@ -4190,7 +4290,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="14.25" customHeight="1">
       <c r="A19" s="35" t="s">
         <v>95</v>
       </c>
@@ -4201,7 +4301,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="14.25" customHeight="1">
       <c r="B20" s="35" t="s">
         <v>98</v>
       </c>
@@ -4221,7 +4321,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="14.25" customHeight="1">
       <c r="B21" s="35" t="s">
         <v>104</v>
       </c>
@@ -4241,7 +4341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="14.25" customHeight="1">
       <c r="B22" s="35" t="s">
         <v>105</v>
       </c>
@@ -4261,7 +4361,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="14.25" customHeight="1">
       <c r="J23" s="38"/>
       <c r="K23" s="38"/>
       <c r="P23" s="35" t="s">
@@ -4274,7 +4374,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="14.25" customHeight="1">
       <c r="J24" s="38"/>
       <c r="K24" s="38"/>
       <c r="P24" s="35">
@@ -4287,7 +4387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="14.25" customHeight="1">
       <c r="D25" s="35" t="s">
         <v>111</v>
       </c>
@@ -4301,7 +4401,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="14.25" customHeight="1">
       <c r="E26" s="35" t="s">
         <v>114</v>
       </c>
@@ -4312,980 +4412,980 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:19" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:19" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:19" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:19" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:19" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:19" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.25" customHeight="1"/>
+    <row r="66" ht="14.25" customHeight="1"/>
+    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="69" ht="14.25" customHeight="1"/>
+    <row r="70" ht="14.25" customHeight="1"/>
+    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="72" ht="14.25" customHeight="1"/>
+    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="74" ht="14.25" customHeight="1"/>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1"/>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1"/>
+    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="83" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="85" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1"/>
+    <row r="87" ht="14.25" customHeight="1"/>
+    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="89" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1"/>
+    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="93" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1"/>
+    <row r="95" ht="14.25" customHeight="1"/>
+    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="101" ht="14.25" customHeight="1"/>
+    <row r="102" ht="14.25" customHeight="1"/>
+    <row r="103" ht="14.25" customHeight="1"/>
+    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="105" ht="14.25" customHeight="1"/>
+    <row r="106" ht="14.25" customHeight="1"/>
+    <row r="107" ht="14.25" customHeight="1"/>
+    <row r="108" ht="14.25" customHeight="1"/>
+    <row r="109" ht="14.25" customHeight="1"/>
+    <row r="110" ht="14.25" customHeight="1"/>
+    <row r="111" ht="14.25" customHeight="1"/>
+    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="113" ht="14.25" customHeight="1"/>
+    <row r="114" ht="14.25" customHeight="1"/>
+    <row r="115" ht="14.25" customHeight="1"/>
+    <row r="116" ht="14.25" customHeight="1"/>
+    <row r="117" ht="14.25" customHeight="1"/>
+    <row r="118" ht="14.25" customHeight="1"/>
+    <row r="119" ht="14.25" customHeight="1"/>
+    <row r="120" ht="14.25" customHeight="1"/>
+    <row r="121" ht="14.25" customHeight="1"/>
+    <row r="122" ht="14.25" customHeight="1"/>
+    <row r="123" ht="14.25" customHeight="1"/>
+    <row r="124" ht="14.25" customHeight="1"/>
+    <row r="125" ht="14.25" customHeight="1"/>
+    <row r="126" ht="14.25" customHeight="1"/>
+    <row r="127" ht="14.25" customHeight="1"/>
+    <row r="128" ht="14.25" customHeight="1"/>
+    <row r="129" ht="14.25" customHeight="1"/>
+    <row r="130" ht="14.25" customHeight="1"/>
+    <row r="131" ht="14.25" customHeight="1"/>
+    <row r="132" ht="14.25" customHeight="1"/>
+    <row r="133" ht="14.25" customHeight="1"/>
+    <row r="134" ht="14.25" customHeight="1"/>
+    <row r="135" ht="14.25" customHeight="1"/>
+    <row r="136" ht="14.25" customHeight="1"/>
+    <row r="137" ht="14.25" customHeight="1"/>
+    <row r="138" ht="14.25" customHeight="1"/>
+    <row r="139" ht="14.25" customHeight="1"/>
+    <row r="140" ht="14.25" customHeight="1"/>
+    <row r="141" ht="14.25" customHeight="1"/>
+    <row r="142" ht="14.25" customHeight="1"/>
+    <row r="143" ht="14.25" customHeight="1"/>
+    <row r="144" ht="14.25" customHeight="1"/>
+    <row r="145" ht="14.25" customHeight="1"/>
+    <row r="146" ht="14.25" customHeight="1"/>
+    <row r="147" ht="14.25" customHeight="1"/>
+    <row r="148" ht="14.25" customHeight="1"/>
+    <row r="149" ht="14.25" customHeight="1"/>
+    <row r="150" ht="14.25" customHeight="1"/>
+    <row r="151" ht="14.25" customHeight="1"/>
+    <row r="152" ht="14.25" customHeight="1"/>
+    <row r="153" ht="14.25" customHeight="1"/>
+    <row r="154" ht="14.25" customHeight="1"/>
+    <row r="155" ht="14.25" customHeight="1"/>
+    <row r="156" ht="14.25" customHeight="1"/>
+    <row r="157" ht="14.25" customHeight="1"/>
+    <row r="158" ht="14.25" customHeight="1"/>
+    <row r="159" ht="14.25" customHeight="1"/>
+    <row r="160" ht="14.25" customHeight="1"/>
+    <row r="161" ht="14.25" customHeight="1"/>
+    <row r="162" ht="14.25" customHeight="1"/>
+    <row r="163" ht="14.25" customHeight="1"/>
+    <row r="164" ht="14.25" customHeight="1"/>
+    <row r="165" ht="14.25" customHeight="1"/>
+    <row r="166" ht="14.25" customHeight="1"/>
+    <row r="167" ht="14.25" customHeight="1"/>
+    <row r="168" ht="14.25" customHeight="1"/>
+    <row r="169" ht="14.25" customHeight="1"/>
+    <row r="170" ht="14.25" customHeight="1"/>
+    <row r="171" ht="14.25" customHeight="1"/>
+    <row r="172" ht="14.25" customHeight="1"/>
+    <row r="173" ht="14.25" customHeight="1"/>
+    <row r="174" ht="14.25" customHeight="1"/>
+    <row r="175" ht="14.25" customHeight="1"/>
+    <row r="176" ht="14.25" customHeight="1"/>
+    <row r="177" ht="14.25" customHeight="1"/>
+    <row r="178" ht="14.25" customHeight="1"/>
+    <row r="179" ht="14.25" customHeight="1"/>
+    <row r="180" ht="14.25" customHeight="1"/>
+    <row r="181" ht="14.25" customHeight="1"/>
+    <row r="182" ht="14.25" customHeight="1"/>
+    <row r="183" ht="14.25" customHeight="1"/>
+    <row r="184" ht="14.25" customHeight="1"/>
+    <row r="185" ht="14.25" customHeight="1"/>
+    <row r="186" ht="14.25" customHeight="1"/>
+    <row r="187" ht="14.25" customHeight="1"/>
+    <row r="188" ht="14.25" customHeight="1"/>
+    <row r="189" ht="14.25" customHeight="1"/>
+    <row r="190" ht="14.25" customHeight="1"/>
+    <row r="191" ht="14.25" customHeight="1"/>
+    <row r="192" ht="14.25" customHeight="1"/>
+    <row r="193" ht="14.25" customHeight="1"/>
+    <row r="194" ht="14.25" customHeight="1"/>
+    <row r="195" ht="14.25" customHeight="1"/>
+    <row r="196" ht="14.25" customHeight="1"/>
+    <row r="197" ht="14.25" customHeight="1"/>
+    <row r="198" ht="14.25" customHeight="1"/>
+    <row r="199" ht="14.25" customHeight="1"/>
+    <row r="200" ht="14.25" customHeight="1"/>
+    <row r="201" ht="14.25" customHeight="1"/>
+    <row r="202" ht="14.25" customHeight="1"/>
+    <row r="203" ht="14.25" customHeight="1"/>
+    <row r="204" ht="14.25" customHeight="1"/>
+    <row r="205" ht="14.25" customHeight="1"/>
+    <row r="206" ht="14.25" customHeight="1"/>
+    <row r="207" ht="14.25" customHeight="1"/>
+    <row r="208" ht="14.25" customHeight="1"/>
+    <row r="209" ht="14.25" customHeight="1"/>
+    <row r="210" ht="14.25" customHeight="1"/>
+    <row r="211" ht="14.25" customHeight="1"/>
+    <row r="212" ht="14.25" customHeight="1"/>
+    <row r="213" ht="14.25" customHeight="1"/>
+    <row r="214" ht="14.25" customHeight="1"/>
+    <row r="215" ht="14.25" customHeight="1"/>
+    <row r="216" ht="14.25" customHeight="1"/>
+    <row r="217" ht="14.25" customHeight="1"/>
+    <row r="218" ht="14.25" customHeight="1"/>
+    <row r="219" ht="14.25" customHeight="1"/>
+    <row r="220" ht="14.25" customHeight="1"/>
+    <row r="221" ht="14.25" customHeight="1"/>
+    <row r="222" ht="14.25" customHeight="1"/>
+    <row r="223" ht="14.25" customHeight="1"/>
+    <row r="224" ht="14.25" customHeight="1"/>
+    <row r="225" ht="14.25" customHeight="1"/>
+    <row r="226" ht="14.25" customHeight="1"/>
+    <row r="227" ht="14.25" customHeight="1"/>
+    <row r="228" ht="14.25" customHeight="1"/>
+    <row r="229" ht="14.25" customHeight="1"/>
+    <row r="230" ht="14.25" customHeight="1"/>
+    <row r="231" ht="14.25" customHeight="1"/>
+    <row r="232" ht="14.25" customHeight="1"/>
+    <row r="233" ht="14.25" customHeight="1"/>
+    <row r="234" ht="14.25" customHeight="1"/>
+    <row r="235" ht="14.25" customHeight="1"/>
+    <row r="236" ht="14.25" customHeight="1"/>
+    <row r="237" ht="14.25" customHeight="1"/>
+    <row r="238" ht="14.25" customHeight="1"/>
+    <row r="239" ht="14.25" customHeight="1"/>
+    <row r="240" ht="14.25" customHeight="1"/>
+    <row r="241" ht="14.25" customHeight="1"/>
+    <row r="242" ht="14.25" customHeight="1"/>
+    <row r="243" ht="14.25" customHeight="1"/>
+    <row r="244" ht="14.25" customHeight="1"/>
+    <row r="245" ht="14.25" customHeight="1"/>
+    <row r="246" ht="14.25" customHeight="1"/>
+    <row r="247" ht="14.25" customHeight="1"/>
+    <row r="248" ht="14.25" customHeight="1"/>
+    <row r="249" ht="14.25" customHeight="1"/>
+    <row r="250" ht="14.25" customHeight="1"/>
+    <row r="251" ht="14.25" customHeight="1"/>
+    <row r="252" ht="14.25" customHeight="1"/>
+    <row r="253" ht="14.25" customHeight="1"/>
+    <row r="254" ht="14.25" customHeight="1"/>
+    <row r="255" ht="14.25" customHeight="1"/>
+    <row r="256" ht="14.25" customHeight="1"/>
+    <row r="257" ht="14.25" customHeight="1"/>
+    <row r="258" ht="14.25" customHeight="1"/>
+    <row r="259" ht="14.25" customHeight="1"/>
+    <row r="260" ht="14.25" customHeight="1"/>
+    <row r="261" ht="14.25" customHeight="1"/>
+    <row r="262" ht="14.25" customHeight="1"/>
+    <row r="263" ht="14.25" customHeight="1"/>
+    <row r="264" ht="14.25" customHeight="1"/>
+    <row r="265" ht="14.25" customHeight="1"/>
+    <row r="266" ht="14.25" customHeight="1"/>
+    <row r="267" ht="14.25" customHeight="1"/>
+    <row r="268" ht="14.25" customHeight="1"/>
+    <row r="269" ht="14.25" customHeight="1"/>
+    <row r="270" ht="14.25" customHeight="1"/>
+    <row r="271" ht="14.25" customHeight="1"/>
+    <row r="272" ht="14.25" customHeight="1"/>
+    <row r="273" ht="14.25" customHeight="1"/>
+    <row r="274" ht="14.25" customHeight="1"/>
+    <row r="275" ht="14.25" customHeight="1"/>
+    <row r="276" ht="14.25" customHeight="1"/>
+    <row r="277" ht="14.25" customHeight="1"/>
+    <row r="278" ht="14.25" customHeight="1"/>
+    <row r="279" ht="14.25" customHeight="1"/>
+    <row r="280" ht="14.25" customHeight="1"/>
+    <row r="281" ht="14.25" customHeight="1"/>
+    <row r="282" ht="14.25" customHeight="1"/>
+    <row r="283" ht="14.25" customHeight="1"/>
+    <row r="284" ht="14.25" customHeight="1"/>
+    <row r="285" ht="14.25" customHeight="1"/>
+    <row r="286" ht="14.25" customHeight="1"/>
+    <row r="287" ht="14.25" customHeight="1"/>
+    <row r="288" ht="14.25" customHeight="1"/>
+    <row r="289" ht="14.25" customHeight="1"/>
+    <row r="290" ht="14.25" customHeight="1"/>
+    <row r="291" ht="14.25" customHeight="1"/>
+    <row r="292" ht="14.25" customHeight="1"/>
+    <row r="293" ht="14.25" customHeight="1"/>
+    <row r="294" ht="14.25" customHeight="1"/>
+    <row r="295" ht="14.25" customHeight="1"/>
+    <row r="296" ht="14.25" customHeight="1"/>
+    <row r="297" ht="14.25" customHeight="1"/>
+    <row r="298" ht="14.25" customHeight="1"/>
+    <row r="299" ht="14.25" customHeight="1"/>
+    <row r="300" ht="14.25" customHeight="1"/>
+    <row r="301" ht="14.25" customHeight="1"/>
+    <row r="302" ht="14.25" customHeight="1"/>
+    <row r="303" ht="14.25" customHeight="1"/>
+    <row r="304" ht="14.25" customHeight="1"/>
+    <row r="305" ht="14.25" customHeight="1"/>
+    <row r="306" ht="14.25" customHeight="1"/>
+    <row r="307" ht="14.25" customHeight="1"/>
+    <row r="308" ht="14.25" customHeight="1"/>
+    <row r="309" ht="14.25" customHeight="1"/>
+    <row r="310" ht="14.25" customHeight="1"/>
+    <row r="311" ht="14.25" customHeight="1"/>
+    <row r="312" ht="14.25" customHeight="1"/>
+    <row r="313" ht="14.25" customHeight="1"/>
+    <row r="314" ht="14.25" customHeight="1"/>
+    <row r="315" ht="14.25" customHeight="1"/>
+    <row r="316" ht="14.25" customHeight="1"/>
+    <row r="317" ht="14.25" customHeight="1"/>
+    <row r="318" ht="14.25" customHeight="1"/>
+    <row r="319" ht="14.25" customHeight="1"/>
+    <row r="320" ht="14.25" customHeight="1"/>
+    <row r="321" ht="14.25" customHeight="1"/>
+    <row r="322" ht="14.25" customHeight="1"/>
+    <row r="323" ht="14.25" customHeight="1"/>
+    <row r="324" ht="14.25" customHeight="1"/>
+    <row r="325" ht="14.25" customHeight="1"/>
+    <row r="326" ht="14.25" customHeight="1"/>
+    <row r="327" ht="14.25" customHeight="1"/>
+    <row r="328" ht="14.25" customHeight="1"/>
+    <row r="329" ht="14.25" customHeight="1"/>
+    <row r="330" ht="14.25" customHeight="1"/>
+    <row r="331" ht="14.25" customHeight="1"/>
+    <row r="332" ht="14.25" customHeight="1"/>
+    <row r="333" ht="14.25" customHeight="1"/>
+    <row r="334" ht="14.25" customHeight="1"/>
+    <row r="335" ht="14.25" customHeight="1"/>
+    <row r="336" ht="14.25" customHeight="1"/>
+    <row r="337" ht="14.25" customHeight="1"/>
+    <row r="338" ht="14.25" customHeight="1"/>
+    <row r="339" ht="14.25" customHeight="1"/>
+    <row r="340" ht="14.25" customHeight="1"/>
+    <row r="341" ht="14.25" customHeight="1"/>
+    <row r="342" ht="14.25" customHeight="1"/>
+    <row r="343" ht="14.25" customHeight="1"/>
+    <row r="344" ht="14.25" customHeight="1"/>
+    <row r="345" ht="14.25" customHeight="1"/>
+    <row r="346" ht="14.25" customHeight="1"/>
+    <row r="347" ht="14.25" customHeight="1"/>
+    <row r="348" ht="14.25" customHeight="1"/>
+    <row r="349" ht="14.25" customHeight="1"/>
+    <row r="350" ht="14.25" customHeight="1"/>
+    <row r="351" ht="14.25" customHeight="1"/>
+    <row r="352" ht="14.25" customHeight="1"/>
+    <row r="353" ht="14.25" customHeight="1"/>
+    <row r="354" ht="14.25" customHeight="1"/>
+    <row r="355" ht="14.25" customHeight="1"/>
+    <row r="356" ht="14.25" customHeight="1"/>
+    <row r="357" ht="14.25" customHeight="1"/>
+    <row r="358" ht="14.25" customHeight="1"/>
+    <row r="359" ht="14.25" customHeight="1"/>
+    <row r="360" ht="14.25" customHeight="1"/>
+    <row r="361" ht="14.25" customHeight="1"/>
+    <row r="362" ht="14.25" customHeight="1"/>
+    <row r="363" ht="14.25" customHeight="1"/>
+    <row r="364" ht="14.25" customHeight="1"/>
+    <row r="365" ht="14.25" customHeight="1"/>
+    <row r="366" ht="14.25" customHeight="1"/>
+    <row r="367" ht="14.25" customHeight="1"/>
+    <row r="368" ht="14.25" customHeight="1"/>
+    <row r="369" ht="14.25" customHeight="1"/>
+    <row r="370" ht="14.25" customHeight="1"/>
+    <row r="371" ht="14.25" customHeight="1"/>
+    <row r="372" ht="14.25" customHeight="1"/>
+    <row r="373" ht="14.25" customHeight="1"/>
+    <row r="374" ht="14.25" customHeight="1"/>
+    <row r="375" ht="14.25" customHeight="1"/>
+    <row r="376" ht="14.25" customHeight="1"/>
+    <row r="377" ht="14.25" customHeight="1"/>
+    <row r="378" ht="14.25" customHeight="1"/>
+    <row r="379" ht="14.25" customHeight="1"/>
+    <row r="380" ht="14.25" customHeight="1"/>
+    <row r="381" ht="14.25" customHeight="1"/>
+    <row r="382" ht="14.25" customHeight="1"/>
+    <row r="383" ht="14.25" customHeight="1"/>
+    <row r="384" ht="14.25" customHeight="1"/>
+    <row r="385" ht="14.25" customHeight="1"/>
+    <row r="386" ht="14.25" customHeight="1"/>
+    <row r="387" ht="14.25" customHeight="1"/>
+    <row r="388" ht="14.25" customHeight="1"/>
+    <row r="389" ht="14.25" customHeight="1"/>
+    <row r="390" ht="14.25" customHeight="1"/>
+    <row r="391" ht="14.25" customHeight="1"/>
+    <row r="392" ht="14.25" customHeight="1"/>
+    <row r="393" ht="14.25" customHeight="1"/>
+    <row r="394" ht="14.25" customHeight="1"/>
+    <row r="395" ht="14.25" customHeight="1"/>
+    <row r="396" ht="14.25" customHeight="1"/>
+    <row r="397" ht="14.25" customHeight="1"/>
+    <row r="398" ht="14.25" customHeight="1"/>
+    <row r="399" ht="14.25" customHeight="1"/>
+    <row r="400" ht="14.25" customHeight="1"/>
+    <row r="401" ht="14.25" customHeight="1"/>
+    <row r="402" ht="14.25" customHeight="1"/>
+    <row r="403" ht="14.25" customHeight="1"/>
+    <row r="404" ht="14.25" customHeight="1"/>
+    <row r="405" ht="14.25" customHeight="1"/>
+    <row r="406" ht="14.25" customHeight="1"/>
+    <row r="407" ht="14.25" customHeight="1"/>
+    <row r="408" ht="14.25" customHeight="1"/>
+    <row r="409" ht="14.25" customHeight="1"/>
+    <row r="410" ht="14.25" customHeight="1"/>
+    <row r="411" ht="14.25" customHeight="1"/>
+    <row r="412" ht="14.25" customHeight="1"/>
+    <row r="413" ht="14.25" customHeight="1"/>
+    <row r="414" ht="14.25" customHeight="1"/>
+    <row r="415" ht="14.25" customHeight="1"/>
+    <row r="416" ht="14.25" customHeight="1"/>
+    <row r="417" ht="14.25" customHeight="1"/>
+    <row r="418" ht="14.25" customHeight="1"/>
+    <row r="419" ht="14.25" customHeight="1"/>
+    <row r="420" ht="14.25" customHeight="1"/>
+    <row r="421" ht="14.25" customHeight="1"/>
+    <row r="422" ht="14.25" customHeight="1"/>
+    <row r="423" ht="14.25" customHeight="1"/>
+    <row r="424" ht="14.25" customHeight="1"/>
+    <row r="425" ht="14.25" customHeight="1"/>
+    <row r="426" ht="14.25" customHeight="1"/>
+    <row r="427" ht="14.25" customHeight="1"/>
+    <row r="428" ht="14.25" customHeight="1"/>
+    <row r="429" ht="14.25" customHeight="1"/>
+    <row r="430" ht="14.25" customHeight="1"/>
+    <row r="431" ht="14.25" customHeight="1"/>
+    <row r="432" ht="14.25" customHeight="1"/>
+    <row r="433" ht="14.25" customHeight="1"/>
+    <row r="434" ht="14.25" customHeight="1"/>
+    <row r="435" ht="14.25" customHeight="1"/>
+    <row r="436" ht="14.25" customHeight="1"/>
+    <row r="437" ht="14.25" customHeight="1"/>
+    <row r="438" ht="14.25" customHeight="1"/>
+    <row r="439" ht="14.25" customHeight="1"/>
+    <row r="440" ht="14.25" customHeight="1"/>
+    <row r="441" ht="14.25" customHeight="1"/>
+    <row r="442" ht="14.25" customHeight="1"/>
+    <row r="443" ht="14.25" customHeight="1"/>
+    <row r="444" ht="14.25" customHeight="1"/>
+    <row r="445" ht="14.25" customHeight="1"/>
+    <row r="446" ht="14.25" customHeight="1"/>
+    <row r="447" ht="14.25" customHeight="1"/>
+    <row r="448" ht="14.25" customHeight="1"/>
+    <row r="449" ht="14.25" customHeight="1"/>
+    <row r="450" ht="14.25" customHeight="1"/>
+    <row r="451" ht="14.25" customHeight="1"/>
+    <row r="452" ht="14.25" customHeight="1"/>
+    <row r="453" ht="14.25" customHeight="1"/>
+    <row r="454" ht="14.25" customHeight="1"/>
+    <row r="455" ht="14.25" customHeight="1"/>
+    <row r="456" ht="14.25" customHeight="1"/>
+    <row r="457" ht="14.25" customHeight="1"/>
+    <row r="458" ht="14.25" customHeight="1"/>
+    <row r="459" ht="14.25" customHeight="1"/>
+    <row r="460" ht="14.25" customHeight="1"/>
+    <row r="461" ht="14.25" customHeight="1"/>
+    <row r="462" ht="14.25" customHeight="1"/>
+    <row r="463" ht="14.25" customHeight="1"/>
+    <row r="464" ht="14.25" customHeight="1"/>
+    <row r="465" ht="14.25" customHeight="1"/>
+    <row r="466" ht="14.25" customHeight="1"/>
+    <row r="467" ht="14.25" customHeight="1"/>
+    <row r="468" ht="14.25" customHeight="1"/>
+    <row r="469" ht="14.25" customHeight="1"/>
+    <row r="470" ht="14.25" customHeight="1"/>
+    <row r="471" ht="14.25" customHeight="1"/>
+    <row r="472" ht="14.25" customHeight="1"/>
+    <row r="473" ht="14.25" customHeight="1"/>
+    <row r="474" ht="14.25" customHeight="1"/>
+    <row r="475" ht="14.25" customHeight="1"/>
+    <row r="476" ht="14.25" customHeight="1"/>
+    <row r="477" ht="14.25" customHeight="1"/>
+    <row r="478" ht="14.25" customHeight="1"/>
+    <row r="479" ht="14.25" customHeight="1"/>
+    <row r="480" ht="14.25" customHeight="1"/>
+    <row r="481" ht="14.25" customHeight="1"/>
+    <row r="482" ht="14.25" customHeight="1"/>
+    <row r="483" ht="14.25" customHeight="1"/>
+    <row r="484" ht="14.25" customHeight="1"/>
+    <row r="485" ht="14.25" customHeight="1"/>
+    <row r="486" ht="14.25" customHeight="1"/>
+    <row r="487" ht="14.25" customHeight="1"/>
+    <row r="488" ht="14.25" customHeight="1"/>
+    <row r="489" ht="14.25" customHeight="1"/>
+    <row r="490" ht="14.25" customHeight="1"/>
+    <row r="491" ht="14.25" customHeight="1"/>
+    <row r="492" ht="14.25" customHeight="1"/>
+    <row r="493" ht="14.25" customHeight="1"/>
+    <row r="494" ht="14.25" customHeight="1"/>
+    <row r="495" ht="14.25" customHeight="1"/>
+    <row r="496" ht="14.25" customHeight="1"/>
+    <row r="497" ht="14.25" customHeight="1"/>
+    <row r="498" ht="14.25" customHeight="1"/>
+    <row r="499" ht="14.25" customHeight="1"/>
+    <row r="500" ht="14.25" customHeight="1"/>
+    <row r="501" ht="14.25" customHeight="1"/>
+    <row r="502" ht="14.25" customHeight="1"/>
+    <row r="503" ht="14.25" customHeight="1"/>
+    <row r="504" ht="14.25" customHeight="1"/>
+    <row r="505" ht="14.25" customHeight="1"/>
+    <row r="506" ht="14.25" customHeight="1"/>
+    <row r="507" ht="14.25" customHeight="1"/>
+    <row r="508" ht="14.25" customHeight="1"/>
+    <row r="509" ht="14.25" customHeight="1"/>
+    <row r="510" ht="14.25" customHeight="1"/>
+    <row r="511" ht="14.25" customHeight="1"/>
+    <row r="512" ht="14.25" customHeight="1"/>
+    <row r="513" ht="14.25" customHeight="1"/>
+    <row r="514" ht="14.25" customHeight="1"/>
+    <row r="515" ht="14.25" customHeight="1"/>
+    <row r="516" ht="14.25" customHeight="1"/>
+    <row r="517" ht="14.25" customHeight="1"/>
+    <row r="518" ht="14.25" customHeight="1"/>
+    <row r="519" ht="14.25" customHeight="1"/>
+    <row r="520" ht="14.25" customHeight="1"/>
+    <row r="521" ht="14.25" customHeight="1"/>
+    <row r="522" ht="14.25" customHeight="1"/>
+    <row r="523" ht="14.25" customHeight="1"/>
+    <row r="524" ht="14.25" customHeight="1"/>
+    <row r="525" ht="14.25" customHeight="1"/>
+    <row r="526" ht="14.25" customHeight="1"/>
+    <row r="527" ht="14.25" customHeight="1"/>
+    <row r="528" ht="14.25" customHeight="1"/>
+    <row r="529" ht="14.25" customHeight="1"/>
+    <row r="530" ht="14.25" customHeight="1"/>
+    <row r="531" ht="14.25" customHeight="1"/>
+    <row r="532" ht="14.25" customHeight="1"/>
+    <row r="533" ht="14.25" customHeight="1"/>
+    <row r="534" ht="14.25" customHeight="1"/>
+    <row r="535" ht="14.25" customHeight="1"/>
+    <row r="536" ht="14.25" customHeight="1"/>
+    <row r="537" ht="14.25" customHeight="1"/>
+    <row r="538" ht="14.25" customHeight="1"/>
+    <row r="539" ht="14.25" customHeight="1"/>
+    <row r="540" ht="14.25" customHeight="1"/>
+    <row r="541" ht="14.25" customHeight="1"/>
+    <row r="542" ht="14.25" customHeight="1"/>
+    <row r="543" ht="14.25" customHeight="1"/>
+    <row r="544" ht="14.25" customHeight="1"/>
+    <row r="545" ht="14.25" customHeight="1"/>
+    <row r="546" ht="14.25" customHeight="1"/>
+    <row r="547" ht="14.25" customHeight="1"/>
+    <row r="548" ht="14.25" customHeight="1"/>
+    <row r="549" ht="14.25" customHeight="1"/>
+    <row r="550" ht="14.25" customHeight="1"/>
+    <row r="551" ht="14.25" customHeight="1"/>
+    <row r="552" ht="14.25" customHeight="1"/>
+    <row r="553" ht="14.25" customHeight="1"/>
+    <row r="554" ht="14.25" customHeight="1"/>
+    <row r="555" ht="14.25" customHeight="1"/>
+    <row r="556" ht="14.25" customHeight="1"/>
+    <row r="557" ht="14.25" customHeight="1"/>
+    <row r="558" ht="14.25" customHeight="1"/>
+    <row r="559" ht="14.25" customHeight="1"/>
+    <row r="560" ht="14.25" customHeight="1"/>
+    <row r="561" ht="14.25" customHeight="1"/>
+    <row r="562" ht="14.25" customHeight="1"/>
+    <row r="563" ht="14.25" customHeight="1"/>
+    <row r="564" ht="14.25" customHeight="1"/>
+    <row r="565" ht="14.25" customHeight="1"/>
+    <row r="566" ht="14.25" customHeight="1"/>
+    <row r="567" ht="14.25" customHeight="1"/>
+    <row r="568" ht="14.25" customHeight="1"/>
+    <row r="569" ht="14.25" customHeight="1"/>
+    <row r="570" ht="14.25" customHeight="1"/>
+    <row r="571" ht="14.25" customHeight="1"/>
+    <row r="572" ht="14.25" customHeight="1"/>
+    <row r="573" ht="14.25" customHeight="1"/>
+    <row r="574" ht="14.25" customHeight="1"/>
+    <row r="575" ht="14.25" customHeight="1"/>
+    <row r="576" ht="14.25" customHeight="1"/>
+    <row r="577" ht="14.25" customHeight="1"/>
+    <row r="578" ht="14.25" customHeight="1"/>
+    <row r="579" ht="14.25" customHeight="1"/>
+    <row r="580" ht="14.25" customHeight="1"/>
+    <row r="581" ht="14.25" customHeight="1"/>
+    <row r="582" ht="14.25" customHeight="1"/>
+    <row r="583" ht="14.25" customHeight="1"/>
+    <row r="584" ht="14.25" customHeight="1"/>
+    <row r="585" ht="14.25" customHeight="1"/>
+    <row r="586" ht="14.25" customHeight="1"/>
+    <row r="587" ht="14.25" customHeight="1"/>
+    <row r="588" ht="14.25" customHeight="1"/>
+    <row r="589" ht="14.25" customHeight="1"/>
+    <row r="590" ht="14.25" customHeight="1"/>
+    <row r="591" ht="14.25" customHeight="1"/>
+    <row r="592" ht="14.25" customHeight="1"/>
+    <row r="593" ht="14.25" customHeight="1"/>
+    <row r="594" ht="14.25" customHeight="1"/>
+    <row r="595" ht="14.25" customHeight="1"/>
+    <row r="596" ht="14.25" customHeight="1"/>
+    <row r="597" ht="14.25" customHeight="1"/>
+    <row r="598" ht="14.25" customHeight="1"/>
+    <row r="599" ht="14.25" customHeight="1"/>
+    <row r="600" ht="14.25" customHeight="1"/>
+    <row r="601" ht="14.25" customHeight="1"/>
+    <row r="602" ht="14.25" customHeight="1"/>
+    <row r="603" ht="14.25" customHeight="1"/>
+    <row r="604" ht="14.25" customHeight="1"/>
+    <row r="605" ht="14.25" customHeight="1"/>
+    <row r="606" ht="14.25" customHeight="1"/>
+    <row r="607" ht="14.25" customHeight="1"/>
+    <row r="608" ht="14.25" customHeight="1"/>
+    <row r="609" ht="14.25" customHeight="1"/>
+    <row r="610" ht="14.25" customHeight="1"/>
+    <row r="611" ht="14.25" customHeight="1"/>
+    <row r="612" ht="14.25" customHeight="1"/>
+    <row r="613" ht="14.25" customHeight="1"/>
+    <row r="614" ht="14.25" customHeight="1"/>
+    <row r="615" ht="14.25" customHeight="1"/>
+    <row r="616" ht="14.25" customHeight="1"/>
+    <row r="617" ht="14.25" customHeight="1"/>
+    <row r="618" ht="14.25" customHeight="1"/>
+    <row r="619" ht="14.25" customHeight="1"/>
+    <row r="620" ht="14.25" customHeight="1"/>
+    <row r="621" ht="14.25" customHeight="1"/>
+    <row r="622" ht="14.25" customHeight="1"/>
+    <row r="623" ht="14.25" customHeight="1"/>
+    <row r="624" ht="14.25" customHeight="1"/>
+    <row r="625" ht="14.25" customHeight="1"/>
+    <row r="626" ht="14.25" customHeight="1"/>
+    <row r="627" ht="14.25" customHeight="1"/>
+    <row r="628" ht="14.25" customHeight="1"/>
+    <row r="629" ht="14.25" customHeight="1"/>
+    <row r="630" ht="14.25" customHeight="1"/>
+    <row r="631" ht="14.25" customHeight="1"/>
+    <row r="632" ht="14.25" customHeight="1"/>
+    <row r="633" ht="14.25" customHeight="1"/>
+    <row r="634" ht="14.25" customHeight="1"/>
+    <row r="635" ht="14.25" customHeight="1"/>
+    <row r="636" ht="14.25" customHeight="1"/>
+    <row r="637" ht="14.25" customHeight="1"/>
+    <row r="638" ht="14.25" customHeight="1"/>
+    <row r="639" ht="14.25" customHeight="1"/>
+    <row r="640" ht="14.25" customHeight="1"/>
+    <row r="641" ht="14.25" customHeight="1"/>
+    <row r="642" ht="14.25" customHeight="1"/>
+    <row r="643" ht="14.25" customHeight="1"/>
+    <row r="644" ht="14.25" customHeight="1"/>
+    <row r="645" ht="14.25" customHeight="1"/>
+    <row r="646" ht="14.25" customHeight="1"/>
+    <row r="647" ht="14.25" customHeight="1"/>
+    <row r="648" ht="14.25" customHeight="1"/>
+    <row r="649" ht="14.25" customHeight="1"/>
+    <row r="650" ht="14.25" customHeight="1"/>
+    <row r="651" ht="14.25" customHeight="1"/>
+    <row r="652" ht="14.25" customHeight="1"/>
+    <row r="653" ht="14.25" customHeight="1"/>
+    <row r="654" ht="14.25" customHeight="1"/>
+    <row r="655" ht="14.25" customHeight="1"/>
+    <row r="656" ht="14.25" customHeight="1"/>
+    <row r="657" ht="14.25" customHeight="1"/>
+    <row r="658" ht="14.25" customHeight="1"/>
+    <row r="659" ht="14.25" customHeight="1"/>
+    <row r="660" ht="14.25" customHeight="1"/>
+    <row r="661" ht="14.25" customHeight="1"/>
+    <row r="662" ht="14.25" customHeight="1"/>
+    <row r="663" ht="14.25" customHeight="1"/>
+    <row r="664" ht="14.25" customHeight="1"/>
+    <row r="665" ht="14.25" customHeight="1"/>
+    <row r="666" ht="14.25" customHeight="1"/>
+    <row r="667" ht="14.25" customHeight="1"/>
+    <row r="668" ht="14.25" customHeight="1"/>
+    <row r="669" ht="14.25" customHeight="1"/>
+    <row r="670" ht="14.25" customHeight="1"/>
+    <row r="671" ht="14.25" customHeight="1"/>
+    <row r="672" ht="14.25" customHeight="1"/>
+    <row r="673" ht="14.25" customHeight="1"/>
+    <row r="674" ht="14.25" customHeight="1"/>
+    <row r="675" ht="14.25" customHeight="1"/>
+    <row r="676" ht="14.25" customHeight="1"/>
+    <row r="677" ht="14.25" customHeight="1"/>
+    <row r="678" ht="14.25" customHeight="1"/>
+    <row r="679" ht="14.25" customHeight="1"/>
+    <row r="680" ht="14.25" customHeight="1"/>
+    <row r="681" ht="14.25" customHeight="1"/>
+    <row r="682" ht="14.25" customHeight="1"/>
+    <row r="683" ht="14.25" customHeight="1"/>
+    <row r="684" ht="14.25" customHeight="1"/>
+    <row r="685" ht="14.25" customHeight="1"/>
+    <row r="686" ht="14.25" customHeight="1"/>
+    <row r="687" ht="14.25" customHeight="1"/>
+    <row r="688" ht="14.25" customHeight="1"/>
+    <row r="689" ht="14.25" customHeight="1"/>
+    <row r="690" ht="14.25" customHeight="1"/>
+    <row r="691" ht="14.25" customHeight="1"/>
+    <row r="692" ht="14.25" customHeight="1"/>
+    <row r="693" ht="14.25" customHeight="1"/>
+    <row r="694" ht="14.25" customHeight="1"/>
+    <row r="695" ht="14.25" customHeight="1"/>
+    <row r="696" ht="14.25" customHeight="1"/>
+    <row r="697" ht="14.25" customHeight="1"/>
+    <row r="698" ht="14.25" customHeight="1"/>
+    <row r="699" ht="14.25" customHeight="1"/>
+    <row r="700" ht="14.25" customHeight="1"/>
+    <row r="701" ht="14.25" customHeight="1"/>
+    <row r="702" ht="14.25" customHeight="1"/>
+    <row r="703" ht="14.25" customHeight="1"/>
+    <row r="704" ht="14.25" customHeight="1"/>
+    <row r="705" ht="14.25" customHeight="1"/>
+    <row r="706" ht="14.25" customHeight="1"/>
+    <row r="707" ht="14.25" customHeight="1"/>
+    <row r="708" ht="14.25" customHeight="1"/>
+    <row r="709" ht="14.25" customHeight="1"/>
+    <row r="710" ht="14.25" customHeight="1"/>
+    <row r="711" ht="14.25" customHeight="1"/>
+    <row r="712" ht="14.25" customHeight="1"/>
+    <row r="713" ht="14.25" customHeight="1"/>
+    <row r="714" ht="14.25" customHeight="1"/>
+    <row r="715" ht="14.25" customHeight="1"/>
+    <row r="716" ht="14.25" customHeight="1"/>
+    <row r="717" ht="14.25" customHeight="1"/>
+    <row r="718" ht="14.25" customHeight="1"/>
+    <row r="719" ht="14.25" customHeight="1"/>
+    <row r="720" ht="14.25" customHeight="1"/>
+    <row r="721" ht="14.25" customHeight="1"/>
+    <row r="722" ht="14.25" customHeight="1"/>
+    <row r="723" ht="14.25" customHeight="1"/>
+    <row r="724" ht="14.25" customHeight="1"/>
+    <row r="725" ht="14.25" customHeight="1"/>
+    <row r="726" ht="14.25" customHeight="1"/>
+    <row r="727" ht="14.25" customHeight="1"/>
+    <row r="728" ht="14.25" customHeight="1"/>
+    <row r="729" ht="14.25" customHeight="1"/>
+    <row r="730" ht="14.25" customHeight="1"/>
+    <row r="731" ht="14.25" customHeight="1"/>
+    <row r="732" ht="14.25" customHeight="1"/>
+    <row r="733" ht="14.25" customHeight="1"/>
+    <row r="734" ht="14.25" customHeight="1"/>
+    <row r="735" ht="14.25" customHeight="1"/>
+    <row r="736" ht="14.25" customHeight="1"/>
+    <row r="737" ht="14.25" customHeight="1"/>
+    <row r="738" ht="14.25" customHeight="1"/>
+    <row r="739" ht="14.25" customHeight="1"/>
+    <row r="740" ht="14.25" customHeight="1"/>
+    <row r="741" ht="14.25" customHeight="1"/>
+    <row r="742" ht="14.25" customHeight="1"/>
+    <row r="743" ht="14.25" customHeight="1"/>
+    <row r="744" ht="14.25" customHeight="1"/>
+    <row r="745" ht="14.25" customHeight="1"/>
+    <row r="746" ht="14.25" customHeight="1"/>
+    <row r="747" ht="14.25" customHeight="1"/>
+    <row r="748" ht="14.25" customHeight="1"/>
+    <row r="749" ht="14.25" customHeight="1"/>
+    <row r="750" ht="14.25" customHeight="1"/>
+    <row r="751" ht="14.25" customHeight="1"/>
+    <row r="752" ht="14.25" customHeight="1"/>
+    <row r="753" ht="14.25" customHeight="1"/>
+    <row r="754" ht="14.25" customHeight="1"/>
+    <row r="755" ht="14.25" customHeight="1"/>
+    <row r="756" ht="14.25" customHeight="1"/>
+    <row r="757" ht="14.25" customHeight="1"/>
+    <row r="758" ht="14.25" customHeight="1"/>
+    <row r="759" ht="14.25" customHeight="1"/>
+    <row r="760" ht="14.25" customHeight="1"/>
+    <row r="761" ht="14.25" customHeight="1"/>
+    <row r="762" ht="14.25" customHeight="1"/>
+    <row r="763" ht="14.25" customHeight="1"/>
+    <row r="764" ht="14.25" customHeight="1"/>
+    <row r="765" ht="14.25" customHeight="1"/>
+    <row r="766" ht="14.25" customHeight="1"/>
+    <row r="767" ht="14.25" customHeight="1"/>
+    <row r="768" ht="14.25" customHeight="1"/>
+    <row r="769" ht="14.25" customHeight="1"/>
+    <row r="770" ht="14.25" customHeight="1"/>
+    <row r="771" ht="14.25" customHeight="1"/>
+    <row r="772" ht="14.25" customHeight="1"/>
+    <row r="773" ht="14.25" customHeight="1"/>
+    <row r="774" ht="14.25" customHeight="1"/>
+    <row r="775" ht="14.25" customHeight="1"/>
+    <row r="776" ht="14.25" customHeight="1"/>
+    <row r="777" ht="14.25" customHeight="1"/>
+    <row r="778" ht="14.25" customHeight="1"/>
+    <row r="779" ht="14.25" customHeight="1"/>
+    <row r="780" ht="14.25" customHeight="1"/>
+    <row r="781" ht="14.25" customHeight="1"/>
+    <row r="782" ht="14.25" customHeight="1"/>
+    <row r="783" ht="14.25" customHeight="1"/>
+    <row r="784" ht="14.25" customHeight="1"/>
+    <row r="785" ht="14.25" customHeight="1"/>
+    <row r="786" ht="14.25" customHeight="1"/>
+    <row r="787" ht="14.25" customHeight="1"/>
+    <row r="788" ht="14.25" customHeight="1"/>
+    <row r="789" ht="14.25" customHeight="1"/>
+    <row r="790" ht="14.25" customHeight="1"/>
+    <row r="791" ht="14.25" customHeight="1"/>
+    <row r="792" ht="14.25" customHeight="1"/>
+    <row r="793" ht="14.25" customHeight="1"/>
+    <row r="794" ht="14.25" customHeight="1"/>
+    <row r="795" ht="14.25" customHeight="1"/>
+    <row r="796" ht="14.25" customHeight="1"/>
+    <row r="797" ht="14.25" customHeight="1"/>
+    <row r="798" ht="14.25" customHeight="1"/>
+    <row r="799" ht="14.25" customHeight="1"/>
+    <row r="800" ht="14.25" customHeight="1"/>
+    <row r="801" ht="14.25" customHeight="1"/>
+    <row r="802" ht="14.25" customHeight="1"/>
+    <row r="803" ht="14.25" customHeight="1"/>
+    <row r="804" ht="14.25" customHeight="1"/>
+    <row r="805" ht="14.25" customHeight="1"/>
+    <row r="806" ht="14.25" customHeight="1"/>
+    <row r="807" ht="14.25" customHeight="1"/>
+    <row r="808" ht="14.25" customHeight="1"/>
+    <row r="809" ht="14.25" customHeight="1"/>
+    <row r="810" ht="14.25" customHeight="1"/>
+    <row r="811" ht="14.25" customHeight="1"/>
+    <row r="812" ht="14.25" customHeight="1"/>
+    <row r="813" ht="14.25" customHeight="1"/>
+    <row r="814" ht="14.25" customHeight="1"/>
+    <row r="815" ht="14.25" customHeight="1"/>
+    <row r="816" ht="14.25" customHeight="1"/>
+    <row r="817" ht="14.25" customHeight="1"/>
+    <row r="818" ht="14.25" customHeight="1"/>
+    <row r="819" ht="14.25" customHeight="1"/>
+    <row r="820" ht="14.25" customHeight="1"/>
+    <row r="821" ht="14.25" customHeight="1"/>
+    <row r="822" ht="14.25" customHeight="1"/>
+    <row r="823" ht="14.25" customHeight="1"/>
+    <row r="824" ht="14.25" customHeight="1"/>
+    <row r="825" ht="14.25" customHeight="1"/>
+    <row r="826" ht="14.25" customHeight="1"/>
+    <row r="827" ht="14.25" customHeight="1"/>
+    <row r="828" ht="14.25" customHeight="1"/>
+    <row r="829" ht="14.25" customHeight="1"/>
+    <row r="830" ht="14.25" customHeight="1"/>
+    <row r="831" ht="14.25" customHeight="1"/>
+    <row r="832" ht="14.25" customHeight="1"/>
+    <row r="833" ht="14.25" customHeight="1"/>
+    <row r="834" ht="14.25" customHeight="1"/>
+    <row r="835" ht="14.25" customHeight="1"/>
+    <row r="836" ht="14.25" customHeight="1"/>
+    <row r="837" ht="14.25" customHeight="1"/>
+    <row r="838" ht="14.25" customHeight="1"/>
+    <row r="839" ht="14.25" customHeight="1"/>
+    <row r="840" ht="14.25" customHeight="1"/>
+    <row r="841" ht="14.25" customHeight="1"/>
+    <row r="842" ht="14.25" customHeight="1"/>
+    <row r="843" ht="14.25" customHeight="1"/>
+    <row r="844" ht="14.25" customHeight="1"/>
+    <row r="845" ht="14.25" customHeight="1"/>
+    <row r="846" ht="14.25" customHeight="1"/>
+    <row r="847" ht="14.25" customHeight="1"/>
+    <row r="848" ht="14.25" customHeight="1"/>
+    <row r="849" ht="14.25" customHeight="1"/>
+    <row r="850" ht="14.25" customHeight="1"/>
+    <row r="851" ht="14.25" customHeight="1"/>
+    <row r="852" ht="14.25" customHeight="1"/>
+    <row r="853" ht="14.25" customHeight="1"/>
+    <row r="854" ht="14.25" customHeight="1"/>
+    <row r="855" ht="14.25" customHeight="1"/>
+    <row r="856" ht="14.25" customHeight="1"/>
+    <row r="857" ht="14.25" customHeight="1"/>
+    <row r="858" ht="14.25" customHeight="1"/>
+    <row r="859" ht="14.25" customHeight="1"/>
+    <row r="860" ht="14.25" customHeight="1"/>
+    <row r="861" ht="14.25" customHeight="1"/>
+    <row r="862" ht="14.25" customHeight="1"/>
+    <row r="863" ht="14.25" customHeight="1"/>
+    <row r="864" ht="14.25" customHeight="1"/>
+    <row r="865" ht="14.25" customHeight="1"/>
+    <row r="866" ht="14.25" customHeight="1"/>
+    <row r="867" ht="14.25" customHeight="1"/>
+    <row r="868" ht="14.25" customHeight="1"/>
+    <row r="869" ht="14.25" customHeight="1"/>
+    <row r="870" ht="14.25" customHeight="1"/>
+    <row r="871" ht="14.25" customHeight="1"/>
+    <row r="872" ht="14.25" customHeight="1"/>
+    <row r="873" ht="14.25" customHeight="1"/>
+    <row r="874" ht="14.25" customHeight="1"/>
+    <row r="875" ht="14.25" customHeight="1"/>
+    <row r="876" ht="14.25" customHeight="1"/>
+    <row r="877" ht="14.25" customHeight="1"/>
+    <row r="878" ht="14.25" customHeight="1"/>
+    <row r="879" ht="14.25" customHeight="1"/>
+    <row r="880" ht="14.25" customHeight="1"/>
+    <row r="881" ht="14.25" customHeight="1"/>
+    <row r="882" ht="14.25" customHeight="1"/>
+    <row r="883" ht="14.25" customHeight="1"/>
+    <row r="884" ht="14.25" customHeight="1"/>
+    <row r="885" ht="14.25" customHeight="1"/>
+    <row r="886" ht="14.25" customHeight="1"/>
+    <row r="887" ht="14.25" customHeight="1"/>
+    <row r="888" ht="14.25" customHeight="1"/>
+    <row r="889" ht="14.25" customHeight="1"/>
+    <row r="890" ht="14.25" customHeight="1"/>
+    <row r="891" ht="14.25" customHeight="1"/>
+    <row r="892" ht="14.25" customHeight="1"/>
+    <row r="893" ht="14.25" customHeight="1"/>
+    <row r="894" ht="14.25" customHeight="1"/>
+    <row r="895" ht="14.25" customHeight="1"/>
+    <row r="896" ht="14.25" customHeight="1"/>
+    <row r="897" ht="14.25" customHeight="1"/>
+    <row r="898" ht="14.25" customHeight="1"/>
+    <row r="899" ht="14.25" customHeight="1"/>
+    <row r="900" ht="14.25" customHeight="1"/>
+    <row r="901" ht="14.25" customHeight="1"/>
+    <row r="902" ht="14.25" customHeight="1"/>
+    <row r="903" ht="14.25" customHeight="1"/>
+    <row r="904" ht="14.25" customHeight="1"/>
+    <row r="905" ht="14.25" customHeight="1"/>
+    <row r="906" ht="14.25" customHeight="1"/>
+    <row r="907" ht="14.25" customHeight="1"/>
+    <row r="908" ht="14.25" customHeight="1"/>
+    <row r="909" ht="14.25" customHeight="1"/>
+    <row r="910" ht="14.25" customHeight="1"/>
+    <row r="911" ht="14.25" customHeight="1"/>
+    <row r="912" ht="14.25" customHeight="1"/>
+    <row r="913" ht="14.25" customHeight="1"/>
+    <row r="914" ht="14.25" customHeight="1"/>
+    <row r="915" ht="14.25" customHeight="1"/>
+    <row r="916" ht="14.25" customHeight="1"/>
+    <row r="917" ht="14.25" customHeight="1"/>
+    <row r="918" ht="14.25" customHeight="1"/>
+    <row r="919" ht="14.25" customHeight="1"/>
+    <row r="920" ht="14.25" customHeight="1"/>
+    <row r="921" ht="14.25" customHeight="1"/>
+    <row r="922" ht="14.25" customHeight="1"/>
+    <row r="923" ht="14.25" customHeight="1"/>
+    <row r="924" ht="14.25" customHeight="1"/>
+    <row r="925" ht="14.25" customHeight="1"/>
+    <row r="926" ht="14.25" customHeight="1"/>
+    <row r="927" ht="14.25" customHeight="1"/>
+    <row r="928" ht="14.25" customHeight="1"/>
+    <row r="929" ht="14.25" customHeight="1"/>
+    <row r="930" ht="14.25" customHeight="1"/>
+    <row r="931" ht="14.25" customHeight="1"/>
+    <row r="932" ht="14.25" customHeight="1"/>
+    <row r="933" ht="14.25" customHeight="1"/>
+    <row r="934" ht="14.25" customHeight="1"/>
+    <row r="935" ht="14.25" customHeight="1"/>
+    <row r="936" ht="14.25" customHeight="1"/>
+    <row r="937" ht="14.25" customHeight="1"/>
+    <row r="938" ht="14.25" customHeight="1"/>
+    <row r="939" ht="14.25" customHeight="1"/>
+    <row r="940" ht="14.25" customHeight="1"/>
+    <row r="941" ht="14.25" customHeight="1"/>
+    <row r="942" ht="14.25" customHeight="1"/>
+    <row r="943" ht="14.25" customHeight="1"/>
+    <row r="944" ht="14.25" customHeight="1"/>
+    <row r="945" ht="14.25" customHeight="1"/>
+    <row r="946" ht="14.25" customHeight="1"/>
+    <row r="947" ht="14.25" customHeight="1"/>
+    <row r="948" ht="14.25" customHeight="1"/>
+    <row r="949" ht="14.25" customHeight="1"/>
+    <row r="950" ht="14.25" customHeight="1"/>
+    <row r="951" ht="14.25" customHeight="1"/>
+    <row r="952" ht="14.25" customHeight="1"/>
+    <row r="953" ht="14.25" customHeight="1"/>
+    <row r="954" ht="14.25" customHeight="1"/>
+    <row r="955" ht="14.25" customHeight="1"/>
+    <row r="956" ht="14.25" customHeight="1"/>
+    <row r="957" ht="14.25" customHeight="1"/>
+    <row r="958" ht="14.25" customHeight="1"/>
+    <row r="959" ht="14.25" customHeight="1"/>
+    <row r="960" ht="14.25" customHeight="1"/>
+    <row r="961" ht="14.25" customHeight="1"/>
+    <row r="962" ht="14.25" customHeight="1"/>
+    <row r="963" ht="14.25" customHeight="1"/>
+    <row r="964" ht="14.25" customHeight="1"/>
+    <row r="965" ht="14.25" customHeight="1"/>
+    <row r="966" ht="14.25" customHeight="1"/>
+    <row r="967" ht="14.25" customHeight="1"/>
+    <row r="968" ht="14.25" customHeight="1"/>
+    <row r="969" ht="14.25" customHeight="1"/>
+    <row r="970" ht="14.25" customHeight="1"/>
+    <row r="971" ht="14.25" customHeight="1"/>
+    <row r="972" ht="14.25" customHeight="1"/>
+    <row r="973" ht="14.25" customHeight="1"/>
+    <row r="974" ht="14.25" customHeight="1"/>
+    <row r="975" ht="14.25" customHeight="1"/>
+    <row r="976" ht="14.25" customHeight="1"/>
+    <row r="977" ht="14.25" customHeight="1"/>
+    <row r="978" ht="14.25" customHeight="1"/>
+    <row r="979" ht="14.25" customHeight="1"/>
+    <row r="980" ht="14.25" customHeight="1"/>
+    <row r="981" ht="14.25" customHeight="1"/>
+    <row r="982" ht="14.25" customHeight="1"/>
+    <row r="983" ht="14.25" customHeight="1"/>
+    <row r="984" ht="14.25" customHeight="1"/>
+    <row r="985" ht="14.25" customHeight="1"/>
+    <row r="986" ht="14.25" customHeight="1"/>
+    <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
+    <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>